<commit_message>
Adding loadedViews into memory
</commit_message>
<xml_diff>
--- a/docs/allocation.xlsx
+++ b/docs/allocation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Version\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C6C265-48C3-451E-90CB-CDABD07BC853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED4543C-9614-4D80-A4A1-62EBB6860344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="16000" yWindow="5110" windowWidth="3560" windowHeight="5440" activeTab="4" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" activeTab="2" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="44">
   <si>
     <t>Type</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t>viewTab</t>
+  </si>
+  <si>
+    <t>loadedView</t>
   </si>
 </sst>
 </file>
@@ -895,8 +898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A86A6CAE-A2FB-4700-AF3B-F451BF94FBFE}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -981,13 +984,32 @@
         <v>840</v>
       </c>
     </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5">
+        <f>B4+ E4+1</f>
+        <v>4623</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>256</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ref="E5" si="3">C5*D5</f>
+        <v>1536</v>
+      </c>
+    </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E13">
         <f>SUM(E2:E11)</f>
-        <v>4620</v>
+        <v>6156</v>
       </c>
     </row>
   </sheetData>
@@ -1199,7 +1221,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF57E188-51E7-49EE-9F4F-07D9A5354CD1}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed bug causing crash when view loaded Also bug causing code length to be calculated on view like it was a logic file
</commit_message>
<xml_diff>
--- a/docs/allocation.xlsx
+++ b/docs/allocation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED4543C-9614-4D80-A4A1-62EBB6860344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF4AE0B-5006-482E-81FA-40254160BA83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" activeTab="2" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
@@ -899,7 +899,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
No loading number of loops and cells
</commit_message>
<xml_diff>
--- a/docs/allocation.xlsx
+++ b/docs/allocation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF4AE0B-5006-482E-81FA-40254160BA83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D1B6BB-2E0D-4488-82B1-97EF377F8153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" activeTab="2" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
@@ -899,7 +899,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -993,14 +993,14 @@
         <v>4623</v>
       </c>
       <c r="C5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D5">
         <v>256</v>
       </c>
       <c r="E5">
         <f t="shared" ref="E5" si="3">C5*D5</f>
-        <v>1536</v>
+        <v>1792</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -1009,7 +1009,7 @@
       </c>
       <c r="E13">
         <f>SUM(E2:E11)</f>
-        <v>6156</v>
+        <v>6412</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed issue causing crash on call of blit, and no view object to be updated
</commit_message>
<xml_diff>
--- a/docs/allocation.xlsx
+++ b/docs/allocation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D1B6BB-2E0D-4488-82B1-97EF377F8153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A19D5D-02CE-4470-BE4B-6729158E2272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" activeTab="2" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic" sheetId="2" r:id="rId1"/>
@@ -532,7 +532,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{355DE0EA-5B2C-4635-84EE-7D1B81ED29C7}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -898,8 +898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A86A6CAE-A2FB-4700-AF3B-F451BF94FBFE}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -993,14 +993,14 @@
         <v>4623</v>
       </c>
       <c r="C5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D5">
         <v>256</v>
       </c>
       <c r="E5">
         <f t="shared" ref="E5" si="3">C5*D5</f>
-        <v>1792</v>
+        <v>2048</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -1009,7 +1009,7 @@
       </c>
       <c r="E13">
         <f>SUM(E2:E11)</f>
-        <v>6412</v>
+        <v>6668</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixing memory leaks in string functions
</commit_message>
<xml_diff>
--- a/docs/allocation.xlsx
+++ b/docs/allocation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A19D5D-02CE-4470-BE4B-6729158E2272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E59D5B18-17AE-4249-944D-E4EB79904A56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" activeTab="1" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="42">
   <si>
     <t>Type</t>
   </si>
@@ -156,19 +156,13 @@
     <t>getNumTemp</t>
   </si>
   <si>
-    <t>Bank Segment</t>
-  </si>
-  <si>
-    <t>Segments Per Bank</t>
-  </si>
-  <si>
-    <t>Segment Calc</t>
-  </si>
-  <si>
     <t>viewTab</t>
   </si>
   <si>
     <t>loadedView</t>
+  </si>
+  <si>
+    <t>TBD</t>
   </si>
 </sst>
 </file>
@@ -530,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{355DE0EA-5B2C-4635-84EE-7D1B81ED29C7}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -741,32 +735,6 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15">
-        <f>C4/F4</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16">
-        <f>(22-18) * B15 + B14</f>
-        <v>24</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -777,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{382A0DF3-A6E2-4E63-819F-0B238C4B218B}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -827,57 +795,24 @@
       <c r="A3" t="s">
         <v>36</v>
       </c>
-      <c r="B3">
-        <f>B2+ E2+1</f>
-        <v>7043</v>
-      </c>
-      <c r="C3">
-        <v>80</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <f t="shared" ref="E3" si="0">C3*D3</f>
-        <v>80</v>
+      <c r="B3" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>38</v>
       </c>
-      <c r="B4" t="e">
-        <f>#REF! +#REF!+1</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C4">
-        <v>80</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <f t="shared" ref="E4:E5" si="1">C4*D4</f>
-        <v>80</v>
+      <c r="B4" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>37</v>
       </c>
-      <c r="B5" t="e">
-        <f t="shared" ref="B5" si="2">B4+ E4+1</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C5">
-        <v>633</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="1"/>
-        <v>633</v>
+      <c r="B5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -886,7 +821,7 @@
       </c>
       <c r="E12">
         <f>SUM(E2:E10)</f>
-        <v>7835</v>
+        <v>7042</v>
       </c>
     </row>
   </sheetData>
@@ -967,7 +902,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B4">
         <f>B3+ E3+1</f>
@@ -986,7 +921,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B5">
         <f>B4+ E4+1</f>

</xml_diff>

<commit_message>
Tidy and allocation spreadsheet update
</commit_message>
<xml_diff>
--- a/docs/allocation.xlsx
+++ b/docs/allocation.xlsx
@@ -8,16 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E59D5B18-17AE-4249-944D-E4EB79904A56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81277E52-20F9-4CA6-BE9E-258A36B08311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" activeTab="1" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Dynamic" sheetId="2" r:id="rId1"/>
-    <sheet name="Bank3" sheetId="3" r:id="rId2"/>
-    <sheet name="BANK61" sheetId="5" r:id="rId3"/>
-    <sheet name="BANK60" sheetId="1" r:id="rId4"/>
-    <sheet name="Golden" sheetId="4" r:id="rId5"/>
+    <sheet name="Dynamic (Bank 0x10 - 0x27)" sheetId="2" r:id="rId1"/>
+    <sheet name="Bank0x1" sheetId="6" r:id="rId2"/>
+    <sheet name="Bank0x2" sheetId="7" r:id="rId3"/>
+    <sheet name="Bank0x3" sheetId="3" r:id="rId4"/>
+    <sheet name="Bank0x4" sheetId="8" r:id="rId5"/>
+    <sheet name="Bank0x5" sheetId="9" r:id="rId6"/>
+    <sheet name="Bank0x6" sheetId="10" r:id="rId7"/>
+    <sheet name="Bank0x7" sheetId="11" r:id="rId8"/>
+    <sheet name="Bank0x8" sheetId="12" r:id="rId9"/>
+    <sheet name="Bank0x9" sheetId="13" r:id="rId10"/>
+    <sheet name="Bank0xA" sheetId="14" r:id="rId11"/>
+    <sheet name="Bank0xB" sheetId="15" r:id="rId12"/>
+    <sheet name="Bank0xC" sheetId="16" r:id="rId13"/>
+    <sheet name="Bank0xD" sheetId="17" r:id="rId14"/>
+    <sheet name="BANK61" sheetId="5" r:id="rId15"/>
+    <sheet name="BANK60" sheetId="1" r:id="rId16"/>
+    <sheet name="Golden" sheetId="4" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="48">
   <si>
     <t>Type</t>
   </si>
@@ -96,21 +108,6 @@
     <t>soundDir</t>
   </si>
   <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>18-24</t>
-  </si>
-  <si>
-    <t>25-33</t>
-  </si>
-  <si>
-    <t>34-39</t>
-  </si>
-  <si>
     <t>viewDir</t>
   </si>
   <si>
@@ -163,6 +160,39 @@
   </si>
   <si>
     <t>TBD</t>
+  </si>
+  <si>
+    <t>Code Purpose</t>
+  </si>
+  <si>
+    <t>commands.c commands</t>
+  </si>
+  <si>
+    <t>agiFiles.c Load Directories</t>
+  </si>
+  <si>
+    <t>MEKA Main Logic</t>
+  </si>
+  <si>
+    <t>Logic Loading Logic.c</t>
+  </si>
+  <si>
+    <t>View Code</t>
+  </si>
+  <si>
+    <t>0x10</t>
+  </si>
+  <si>
+    <t>0x11</t>
+  </si>
+  <si>
+    <t>0x12-0x18</t>
+  </si>
+  <si>
+    <t>0x19-0x21</t>
+  </si>
+  <si>
+    <t>0x22-0x27</t>
   </si>
 </sst>
 </file>
@@ -526,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{355DE0EA-5B2C-4635-84EE-7D1B81ED29C7}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K24" sqref="K22:K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -582,7 +612,7 @@
         <v>8000</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -609,7 +639,7 @@
         <v>8000</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="F3">
         <f>D3/8000</f>
@@ -639,7 +669,7 @@
         <v>48000</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="F4">
         <f>D4/8000</f>
@@ -669,7 +699,7 @@
         <v>64000</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="F5">
         <f>D5/8000</f>
@@ -699,7 +729,7 @@
         <v>40000</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="F6">
         <f>D6/8000</f>
@@ -741,12 +771,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{382A0DF3-A6E2-4E63-819F-0B238C4B218B}">
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D02A195F-A94B-43B9-B272-B66DEB6E2820}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -754,6 +784,7 @@
     <col min="1" max="1" width="19.81640625" customWidth="1"/>
     <col min="2" max="2" width="6.1796875" customWidth="1"/>
     <col min="3" max="4" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -770,49 +801,31 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>4641</v>
+        <v>3586</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2">
-        <v>7042</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" t="s">
-        <v>41</v>
+        <f>C2</f>
+        <v>3586</v>
+      </c>
+      <c r="F2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -821,7 +834,7 @@
       </c>
       <c r="E12">
         <f>SUM(E2:E10)</f>
-        <v>7042</v>
+        <v>3586</v>
       </c>
     </row>
   </sheetData>
@@ -829,7 +842,290 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B7B0F1E-C979-4C21-B312-FEEDB3E52407}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>5123</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f>C2</f>
+        <v>5123</v>
+      </c>
+      <c r="F2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <f>SUM(E2:E10)</f>
+        <v>5123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E18CACF-38E0-4F05-9197-203383C8FC18}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>3723</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f>C2</f>
+        <v>3723</v>
+      </c>
+      <c r="F2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <f>SUM(E2:E10)</f>
+        <v>3723</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65335C43-E3F8-4707-82AC-D64DB07E5F88}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>5123</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>3093</v>
+      </c>
+      <c r="F2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <f>SUM(E2:E10)</f>
+        <v>3093</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F6CA172-7BA6-40DD-ABB6-E303E9E694A5}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>6127</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f>C2</f>
+        <v>6127</v>
+      </c>
+      <c r="F2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <f>SUM(E2:E10)</f>
+        <v>6127</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A86A6CAE-A2FB-4700-AF3B-F451BF94FBFE}">
   <dimension ref="A1:F13"/>
   <sheetViews>
@@ -858,13 +1154,13 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -882,7 +1178,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B3">
         <f>B2+ E2+1</f>
@@ -902,7 +1198,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B4">
         <f>B3+ E3+1</f>
@@ -921,7 +1217,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B5">
         <f>B4+ E4+1</f>
@@ -953,7 +1249,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8A806B9-8F96-4CFC-8F80-C6046C4BB66C}">
   <dimension ref="A1:F13"/>
   <sheetViews>
@@ -982,7 +1278,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1"/>
     </row>
@@ -1063,7 +1359,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
@@ -1082,7 +1378,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
@@ -1101,7 +1397,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
@@ -1120,7 +1416,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
@@ -1152,7 +1448,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF57E188-51E7-49EE-9F4F-07D9A5354CD1}">
   <dimension ref="A1:E11"/>
   <sheetViews>
@@ -1179,12 +1475,12 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1202,7 +1498,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B3">
         <f>B2+ E2+1</f>
@@ -1221,7 +1517,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B4">
         <f>B3+ E3+1</f>
@@ -1240,7 +1536,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E10">
         <f>SUM(E2:E9)</f>
@@ -1249,7 +1545,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E11">
         <v>1023</v>
@@ -1259,4 +1555,597 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA754253-1AC6-4AC6-91AF-37AC71E22B02}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="21.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>7554</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f>C2</f>
+        <v>7554</v>
+      </c>
+      <c r="F2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <f>SUM(E2:E10)</f>
+        <v>7554</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6700B15-078B-4B8C-B149-C046CE8CC3B4}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="21.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>7663</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f>C2</f>
+        <v>7663</v>
+      </c>
+      <c r="F2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <f>SUM(E2:E10)</f>
+        <v>7663</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{382A0DF3-A6E2-4E63-819F-0B238C4B218B}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="21.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>4641</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f>C2</f>
+        <v>4641</v>
+      </c>
+      <c r="F2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <f>SUM(E2:E10)</f>
+        <v>4641</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4FAB9BB-644E-4DE7-A6F3-2DB946584AF9}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="21.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>4234</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f>C2</f>
+        <v>4234</v>
+      </c>
+      <c r="F2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <f>SUM(E2:E10)</f>
+        <v>4234</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12C5024D-5883-452F-AA38-8CA5B65145D7}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="21.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>6696</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f>C2</f>
+        <v>6696</v>
+      </c>
+      <c r="F2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <f>SUM(E2:E10)</f>
+        <v>6696</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EE80BDF-E657-4A2B-B23B-E05D3D83C462}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="24.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1153</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f>C2</f>
+        <v>1153</v>
+      </c>
+      <c r="F2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <f>SUM(E2:E10)</f>
+        <v>1153</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EED8C9F-5BE2-4E98-B5FC-EB226A731849}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="15.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1645</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f>C2</f>
+        <v>1645</v>
+      </c>
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <f>SUM(E2:E10)</f>
+        <v>1645</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C669B32-4B46-4AD0-A79C-01B618483F1F}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="17.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>516</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f>C2</f>
+        <v>516</v>
+      </c>
+      <c r="F2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <f>SUM(E2:E10)</f>
+        <v>516</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
First draft cache system
</commit_message>
<xml_diff>
--- a/docs/allocation.xlsx
+++ b/docs/allocation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81277E52-20F9-4CA6-BE9E-258A36B08311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A561D93D-CE5C-40FB-A409-F7122597BD85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" firstSheet="1" activeTab="14" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic (Bank 0x10 - 0x27)" sheetId="2" r:id="rId1"/>
@@ -27,9 +27,10 @@
     <sheet name="Bank0xB" sheetId="15" r:id="rId12"/>
     <sheet name="Bank0xC" sheetId="16" r:id="rId13"/>
     <sheet name="Bank0xD" sheetId="17" r:id="rId14"/>
-    <sheet name="BANK61" sheetId="5" r:id="rId15"/>
-    <sheet name="BANK60" sheetId="1" r:id="rId16"/>
-    <sheet name="Golden" sheetId="4" r:id="rId17"/>
+    <sheet name="Bank0xE" sheetId="18" r:id="rId15"/>
+    <sheet name="BANK61" sheetId="5" r:id="rId16"/>
+    <sheet name="BANK60" sheetId="1" r:id="rId17"/>
+    <sheet name="Golden" sheetId="4" r:id="rId18"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="53">
   <si>
     <t>Type</t>
   </si>
@@ -193,6 +194,21 @@
   </si>
   <si>
     <t>0x22-0x27</t>
+  </si>
+  <si>
+    <t>Cache Code</t>
+  </si>
+  <si>
+    <t>lruCache Logic</t>
+  </si>
+  <si>
+    <t>lruCache View</t>
+  </si>
+  <si>
+    <t>lruCache Logic Data</t>
+  </si>
+  <si>
+    <t>IruCache View Data</t>
   </si>
 </sst>
 </file>
@@ -556,7 +572,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{355DE0EA-5B2C-4635-84EE-7D1B81ED29C7}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K24" sqref="K22:K24"/>
     </sheetView>
   </sheetViews>
@@ -1126,11 +1142,158 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1B96CF0-432F-4A3E-940D-86E08F6940C7}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>682</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f>C2</f>
+        <v>682</v>
+      </c>
+      <c r="F2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3">
+        <f>8191 -E3</f>
+        <v>8186</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <f>C3 * D3</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4">
+        <f>B3-E4</f>
+        <v>8176</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <f>C4 * D4</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5">
+        <f>B4-E5</f>
+        <v>8171</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <f>C5 * D5</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6">
+        <f>B5-E6</f>
+        <v>8151</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>20</v>
+      </c>
+      <c r="E6">
+        <f>C6 * D6</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <f>SUM(E2:E10)</f>
+        <v>722</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A86A6CAE-A2FB-4700-AF3B-F451BF94FBFE}">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1249,7 +1412,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8A806B9-8F96-4CFC-8F80-C6046C4BB66C}">
   <dimension ref="A1:F13"/>
   <sheetViews>
@@ -1448,7 +1611,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF57E188-51E7-49EE-9F4F-07D9A5354CD1}">
   <dimension ref="A1:E11"/>
   <sheetViews>

</xml_diff>

<commit_message>
Calling ASM with right params
</commit_message>
<xml_diff>
--- a/docs/allocation.xlsx
+++ b/docs/allocation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8CA1071-82E9-4CAE-8EE4-895FBC392E90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13FC6276-251B-411A-8F63-60F69CC62DAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" firstSheet="1" activeTab="14" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" firstSheet="3" activeTab="17" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic (Bank 0x10 - 0x27)" sheetId="2" r:id="rId1"/>
@@ -37,20 +37,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="54">
   <si>
     <t>Type</t>
   </si>
@@ -209,6 +201,9 @@
   </si>
   <si>
     <t>IruCache View Data</t>
+  </si>
+  <si>
+    <t>parameters</t>
   </si>
 </sst>
 </file>
@@ -562,7 +557,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1145,7 +1140,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1B96CF0-432F-4A3E-940D-86E08F6940C7}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1615,7 +1610,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF57E188-51E7-49EE-9F4F-07D9A5354CD1}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -1697,13 +1692,32 @@
         <v>500</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5">
+        <f>B4+ E4+1</f>
+        <v>1015</v>
+      </c>
+      <c r="C5">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ref="E5" si="2">C5*D5</f>
+        <v>11</v>
+      </c>
+    </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>25</v>
       </c>
       <c r="E10">
         <f>SUM(E2:E9)</f>
-        <v>1012</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Moved execute logic to bank
</commit_message>
<xml_diff>
--- a/docs/allocation.xlsx
+++ b/docs/allocation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13FC6276-251B-411A-8F63-60F69CC62DAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D43DB5-6E4D-4ED2-845D-43D94C6C829F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" firstSheet="3" activeTab="17" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" firstSheet="3" activeTab="7" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic (Bank 0x10 - 0x27)" sheetId="2" r:id="rId1"/>
@@ -164,9 +164,6 @@
     <t>agiFiles.c Load Directories</t>
   </si>
   <si>
-    <t>MEKA Main Logic</t>
-  </si>
-  <si>
     <t>Logic Loading Logic.c</t>
   </si>
   <si>
@@ -204,6 +201,9 @@
   </si>
   <si>
     <t>parameters</t>
+  </si>
+  <si>
+    <t>MEKA Main Logic and execute logic</t>
   </si>
 </sst>
 </file>
@@ -557,7 +557,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -623,7 +623,7 @@
         <v>8000</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -650,7 +650,7 @@
         <v>8000</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F3">
         <f>D3/8000</f>
@@ -680,7 +680,7 @@
         <v>48000</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F4">
         <f>D4/8000</f>
@@ -710,7 +710,7 @@
         <v>64000</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F5">
         <f>D5/8000</f>
@@ -740,7 +740,7 @@
         <v>40000</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F6">
         <f>D6/8000</f>
@@ -836,7 +836,7 @@
         <v>3586</v>
       </c>
       <c r="F2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -907,7 +907,7 @@
         <v>5123</v>
       </c>
       <c r="F2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -978,7 +978,7 @@
         <v>3723</v>
       </c>
       <c r="F2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1048,7 +1048,7 @@
         <v>3093</v>
       </c>
       <c r="F2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1119,7 +1119,7 @@
         <v>6127</v>
       </c>
       <c r="F2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1190,12 +1190,12 @@
         <v>682</v>
       </c>
       <c r="F2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3">
         <f>8191 -E3</f>
@@ -1214,7 +1214,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4">
         <f>B3-E4</f>
@@ -1233,7 +1233,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5">
         <f>B4-E5</f>
@@ -1252,7 +1252,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B6">
         <f>B5-E6</f>
@@ -1610,7 +1610,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF57E188-51E7-49EE-9F4F-07D9A5354CD1}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -1694,7 +1694,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5">
         <f>B4+ E4+1</f>
@@ -2189,8 +2189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EED8C9F-5BE2-4E98-B5FC-EB226A731849}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2198,7 +2198,7 @@
     <col min="1" max="1" width="19.81640625" customWidth="1"/>
     <col min="2" max="2" width="6.1796875" customWidth="1"/>
     <col min="3" max="4" width="11.453125" customWidth="1"/>
-    <col min="6" max="6" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -2229,17 +2229,17 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>1645</v>
+        <v>1789</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2">
         <f>C2</f>
-        <v>1645</v>
+        <v>1789</v>
       </c>
       <c r="F2" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -2248,7 +2248,7 @@
       </c>
       <c r="E12">
         <f>SUM(E2:E10)</f>
-        <v>1645</v>
+        <v>1789</v>
       </c>
     </row>
   </sheetData>
@@ -2310,7 +2310,7 @@
         <v>516</v>
       </c>
       <c r="F2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Reduced memory size by removing malloc and shift char conversion to bank
</commit_message>
<xml_diff>
--- a/docs/allocation.xlsx
+++ b/docs/allocation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4CED546-10FE-4F38-B7E3-4FE0CE7FC764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C51B135-299F-4E4F-8731-DFECD558C4D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" firstSheet="3" activeTab="15" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic (Bank 0x13 - 0x3A)" sheetId="2" r:id="rId1"/>
@@ -28,9 +28,10 @@
     <sheet name="Bank0xC" sheetId="16" r:id="rId13"/>
     <sheet name="Bank0xD" sheetId="17" r:id="rId14"/>
     <sheet name="Bank0xE" sheetId="18" r:id="rId15"/>
-    <sheet name="BANK61" sheetId="5" r:id="rId16"/>
-    <sheet name="BANK60" sheetId="1" r:id="rId17"/>
-    <sheet name="Golden" sheetId="4" r:id="rId18"/>
+    <sheet name="Bank0x10" sheetId="19" r:id="rId16"/>
+    <sheet name="BANK61" sheetId="5" r:id="rId17"/>
+    <sheet name="BANK60" sheetId="1" r:id="rId18"/>
+    <sheet name="Golden" sheetId="4" r:id="rId19"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="57">
   <si>
     <t>Type</t>
   </si>
@@ -204,6 +205,15 @@
   </si>
   <si>
     <t>0x13</t>
+  </si>
+  <si>
+    <t>Memory Management</t>
+  </si>
+  <si>
+    <t>dynamic memory management data</t>
+  </si>
+  <si>
+    <t>memory area</t>
   </si>
 </sst>
 </file>
@@ -567,7 +577,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{355DE0EA-5B2C-4635-84EE-7D1B81ED29C7}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
@@ -1282,6 +1292,95 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C39777F-CEF0-4425-930E-295AE7C473DC}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="31.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="31.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1586</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f>C2</f>
+        <v>1586</v>
+      </c>
+      <c r="F2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3">
+        <v>8156</v>
+      </c>
+      <c r="C3">
+        <v>35</v>
+      </c>
+      <c r="E3">
+        <f>C3</f>
+        <v>35</v>
+      </c>
+      <c r="F3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <f>SUM(E2:E10)</f>
+        <v>1621</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A86A6CAE-A2FB-4700-AF3B-F451BF94FBFE}">
   <dimension ref="A1:F13"/>
   <sheetViews>
@@ -1405,7 +1504,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8A806B9-8F96-4CFC-8F80-C6046C4BB66C}">
   <dimension ref="A1:F13"/>
   <sheetViews>
@@ -1604,7 +1703,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF57E188-51E7-49EE-9F4F-07D9A5354CD1}">
   <dimension ref="A1:E11"/>
   <sheetViews>

</xml_diff>

<commit_message>
Now getting ZP_LE and LF from command loop function in assembler
</commit_message>
<xml_diff>
--- a/docs/allocation.xlsx
+++ b/docs/allocation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C51B135-299F-4E4F-8731-DFECD558C4D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0AE8EBD-BAE2-42DF-AC2D-27534523C75F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" firstSheet="3" activeTab="15" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" firstSheet="3" activeTab="8" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic (Bank 0x13 - 0x3A)" sheetId="2" r:id="rId1"/>
@@ -29,9 +29,10 @@
     <sheet name="Bank0xD" sheetId="17" r:id="rId14"/>
     <sheet name="Bank0xE" sheetId="18" r:id="rId15"/>
     <sheet name="Bank0x10" sheetId="19" r:id="rId16"/>
-    <sheet name="BANK61" sheetId="5" r:id="rId17"/>
-    <sheet name="BANK60" sheetId="1" r:id="rId18"/>
-    <sheet name="Golden" sheetId="4" r:id="rId19"/>
+    <sheet name="BANK60" sheetId="1" r:id="rId17"/>
+    <sheet name="BANK61" sheetId="5" r:id="rId18"/>
+    <sheet name="BANK62" sheetId="20" r:id="rId19"/>
+    <sheet name="Golden" sheetId="4" r:id="rId20"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="59">
   <si>
     <t>Type</t>
   </si>
@@ -214,6 +215,12 @@
   </si>
   <si>
     <t>memory area</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>logicEntryAddresses</t>
   </si>
 </sst>
 </file>
@@ -1295,8 +1302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C39777F-CEF0-4425-930E-295AE7C473DC}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="C7:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1381,6 +1388,205 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8A806B9-8F96-4CFC-8F80-C6046C4BB66C}">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>185</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f>C2*D2</f>
+        <v>185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B9" si="0">B2+ E2+1</f>
+        <v>186</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>255</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E6" si="1">C3*D3</f>
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>1462</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>255</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>2738</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>255</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>4014</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>255</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>5290</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>255</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ref="E7" si="2">C7*D7</f>
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>7331</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>255</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ref="E8" si="3">C8*D8</f>
+        <v>510</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>7842</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>20</v>
+      </c>
+      <c r="E9">
+        <f t="shared" ref="E9" si="4">C9*D9</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <f>SUM(E2:E11)</f>
+        <v>8035</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A86A6CAE-A2FB-4700-AF3B-F451BF94FBFE}">
   <dimension ref="A1:F13"/>
   <sheetViews>
@@ -1489,6 +1695,11 @@
         <v>2048</v>
       </c>
     </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>57</v>
+      </c>
+    </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>2</v>
@@ -1504,12 +1715,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8A806B9-8F96-4CFC-8F80-C6046C4BB66C}">
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1ECB7A9-D68D-4611-9022-3CBE081861CE}">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="A9:E9"/>
+      <selection activeCell="E2" sqref="B2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1539,153 +1750,25 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>185</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>256</v>
       </c>
       <c r="E2">
-        <f>C2*D2</f>
-        <v>185</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3">
-        <f t="shared" ref="B3:B9" si="0">B2+ E2+1</f>
-        <v>186</v>
-      </c>
-      <c r="C3">
-        <v>5</v>
-      </c>
-      <c r="D3">
-        <v>255</v>
-      </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E6" si="1">C3*D3</f>
-        <v>1275</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4">
-        <f t="shared" si="0"/>
-        <v>1462</v>
-      </c>
-      <c r="C4">
-        <v>5</v>
-      </c>
-      <c r="D4">
-        <v>255</v>
-      </c>
-      <c r="E4">
-        <f t="shared" si="1"/>
-        <v>1275</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5">
-        <f t="shared" si="0"/>
-        <v>2738</v>
-      </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-      <c r="D5">
-        <v>255</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="1"/>
-        <v>1275</v>
+        <f t="shared" ref="E2" si="0">C2*D2</f>
+        <v>512</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6">
-        <f t="shared" si="0"/>
-        <v>4014</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-      <c r="D6">
-        <v>255</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="1"/>
-        <v>1275</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7">
-        <f t="shared" si="0"/>
-        <v>5290</v>
-      </c>
-      <c r="C7">
-        <v>8</v>
-      </c>
-      <c r="D7">
-        <v>255</v>
-      </c>
-      <c r="E7">
-        <f t="shared" ref="E7" si="2">C7*D7</f>
-        <v>2040</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8">
-        <f t="shared" si="0"/>
-        <v>7331</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8">
-        <v>255</v>
-      </c>
-      <c r="E8">
-        <f t="shared" ref="E8" si="3">C8*D8</f>
-        <v>510</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9">
-        <f t="shared" si="0"/>
-        <v>7842</v>
-      </c>
-      <c r="C9">
-        <v>10</v>
-      </c>
-      <c r="D9">
-        <v>20</v>
-      </c>
-      <c r="E9">
-        <f t="shared" ref="E9" si="4">C9*D9</f>
-        <v>200</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -1694,135 +1777,7 @@
       </c>
       <c r="E13">
         <f>SUM(E2:E11)</f>
-        <v>8035</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF57E188-51E7-49EE-9F4F-07D9A5354CD1}">
-  <dimension ref="A1:E11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="22.7265625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>256</v>
-      </c>
-      <c r="E2">
-        <f>C2*D2</f>
-        <v>256</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3">
-        <f>B2+ E2+1</f>
-        <v>257</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>256</v>
-      </c>
-      <c r="E3">
-        <f t="shared" ref="E3" si="0">C3*D3</f>
-        <v>256</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4">
-        <f>B3+ E3+1</f>
-        <v>514</v>
-      </c>
-      <c r="C4">
-        <v>500</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <f t="shared" ref="E4" si="1">C4*D4</f>
-        <v>500</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5">
-        <f>B4+ E4+1</f>
-        <v>1015</v>
-      </c>
-      <c r="C5">
-        <v>11</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <f t="shared" ref="E5" si="2">C5*D5</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10">
-        <f>SUM(E2:E9)</f>
-        <v>1023</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11">
-        <v>1023</v>
+        <v>512</v>
       </c>
     </row>
   </sheetData>
@@ -1903,6 +1858,134 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF57E188-51E7-49EE-9F4F-07D9A5354CD1}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="22.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>256</v>
+      </c>
+      <c r="E2">
+        <f>C2*D2</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3">
+        <f>B2+ E2+1</f>
+        <v>257</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>256</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3" si="0">C3*D3</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4">
+        <f>B3+ E3+1</f>
+        <v>514</v>
+      </c>
+      <c r="C4">
+        <v>500</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4" si="1">C4*D4</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5">
+        <f>B4+ E4+1</f>
+        <v>1015</v>
+      </c>
+      <c r="C5">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ref="E5" si="2">C5*D5</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10">
+        <f>SUM(E2:E9)</f>
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11">
+        <v>1023</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6700B15-078B-4B8C-B149-C046CE8CC3B4}">
   <dimension ref="A1:F12"/>
@@ -2357,8 +2440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C669B32-4B46-4AD0-A79C-01B618483F1F}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2410,6 +2493,25 @@
         <v>40</v>
       </c>
     </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11">
+        <f>8191-E11</f>
+        <v>7679</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>256</v>
+      </c>
+      <c r="E11">
+        <f>D11*C11</f>
+        <v>512</v>
+      </c>
+    </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Moving flood counters to low ram
</commit_message>
<xml_diff>
--- a/docs/allocation.xlsx
+++ b/docs/allocation.xlsx
@@ -1,34 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2CA0809-5E5F-423D-A120-6520C7B26FBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497D9927-FCD6-40E5-8C99-BF2C6198649E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" firstSheet="7" activeTab="16" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" firstSheet="8" activeTab="14" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Dynamic (Bank 0x13 - 0x3A)" sheetId="2" r:id="rId1"/>
-    <sheet name="Bank0x1" sheetId="6" r:id="rId2"/>
-    <sheet name="Bank0x2" sheetId="7" r:id="rId3"/>
-    <sheet name="Bank0x3" sheetId="3" r:id="rId4"/>
-    <sheet name="Bank0x4" sheetId="8" r:id="rId5"/>
-    <sheet name="Bank0x5" sheetId="9" r:id="rId6"/>
-    <sheet name="Bank0x6" sheetId="10" r:id="rId7"/>
-    <sheet name="Bank0x7" sheetId="11" r:id="rId8"/>
-    <sheet name="Bank0x8" sheetId="12" r:id="rId9"/>
-    <sheet name="Bank0x9" sheetId="13" r:id="rId10"/>
-    <sheet name="Bank0xA" sheetId="14" r:id="rId11"/>
-    <sheet name="Bank0xB" sheetId="15" r:id="rId12"/>
-    <sheet name="Bank0xC" sheetId="16" r:id="rId13"/>
-    <sheet name="Bank0xD" sheetId="17" r:id="rId14"/>
-    <sheet name="Bank0xE" sheetId="18" r:id="rId15"/>
-    <sheet name="Bank0x10" sheetId="19" r:id="rId16"/>
+    <sheet name="Bank0x1" sheetId="6" r:id="rId1"/>
+    <sheet name="Bank0x2" sheetId="7" r:id="rId2"/>
+    <sheet name="Bank0x3" sheetId="3" r:id="rId3"/>
+    <sheet name="Bank0x4" sheetId="8" r:id="rId4"/>
+    <sheet name="Bank0x5" sheetId="9" r:id="rId5"/>
+    <sheet name="Bank0x6" sheetId="10" r:id="rId6"/>
+    <sheet name="Bank0x7" sheetId="11" r:id="rId7"/>
+    <sheet name="Bank0x8" sheetId="12" r:id="rId8"/>
+    <sheet name="Bank0x9" sheetId="13" r:id="rId9"/>
+    <sheet name="Bank0xA" sheetId="14" r:id="rId10"/>
+    <sheet name="Bank0xB" sheetId="15" r:id="rId11"/>
+    <sheet name="Bank0xC" sheetId="16" r:id="rId12"/>
+    <sheet name="Bank0xD" sheetId="17" r:id="rId13"/>
+    <sheet name="Bank0xE" sheetId="18" r:id="rId14"/>
+    <sheet name="Bank0x10" sheetId="19" r:id="rId15"/>
+    <sheet name="Dynamic (Bank 0x13 - 0x3A)" sheetId="2" r:id="rId16"/>
     <sheet name="BANK0x3C" sheetId="1" r:id="rId17"/>
     <sheet name="BANK0x3D" sheetId="5" r:id="rId18"/>
     <sheet name="BANK0x3E" sheetId="20" r:id="rId19"/>
@@ -581,224 +581,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{355DE0EA-5B2C-4635-84EE-7D1B81ED29C7}">
-  <dimension ref="A1:I9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.1796875" customWidth="1"/>
-    <col min="5" max="5" width="9.453125" customWidth="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.453125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2">
-        <v>100</v>
-      </c>
-      <c r="C2">
-        <v>80</v>
-      </c>
-      <c r="D2">
-        <f>B2*C2</f>
-        <v>8000</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>160</v>
-      </c>
-      <c r="C3">
-        <v>50</v>
-      </c>
-      <c r="D3">
-        <f>B3*C3</f>
-        <v>8000</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F3">
-        <f>D3/8000</f>
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <f>H2+1</f>
-        <v>50</v>
-      </c>
-      <c r="H3">
-        <f>G3+C3 -1</f>
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>1600</v>
-      </c>
-      <c r="C4">
-        <v>30</v>
-      </c>
-      <c r="D4">
-        <f>B4*C4</f>
-        <v>48000</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F4">
-        <v>7</v>
-      </c>
-      <c r="G4">
-        <f>H3+1</f>
-        <v>100</v>
-      </c>
-      <c r="H4">
-        <f>G4+C4 -1</f>
-        <v>129</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>3200</v>
-      </c>
-      <c r="C5">
-        <v>20</v>
-      </c>
-      <c r="D5">
-        <f>B5*C5</f>
-        <v>64000</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F5">
-        <v>9</v>
-      </c>
-      <c r="G5">
-        <f>H4+1</f>
-        <v>130</v>
-      </c>
-      <c r="H5">
-        <f>G5+C5 -1</f>
-        <v>149</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6">
-        <v>8000</v>
-      </c>
-      <c r="C6">
-        <v>6</v>
-      </c>
-      <c r="D6">
-        <f>B6*C6</f>
-        <v>48000</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F6">
-        <f>D6/8000</f>
-        <v>6</v>
-      </c>
-      <c r="G6">
-        <f>H5+1</f>
-        <v>150</v>
-      </c>
-      <c r="H6">
-        <f>G6+C6 - 1</f>
-        <v>155</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9">
-        <f>SUM(B2:B8)</f>
-        <v>13060</v>
-      </c>
-      <c r="C9">
-        <f>SUM(C2:C6)</f>
-        <v>186</v>
-      </c>
-      <c r="D9">
-        <f>SUM(D2:D8)</f>
-        <v>176000</v>
-      </c>
-      <c r="F9">
-        <f>SUM(F2:F6)</f>
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D02A195F-A94B-43B9-B272-B66DEB6E2820}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA754253-1AC6-4AC6-91AF-37AC71E22B02}">
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -810,7 +593,7 @@
     <col min="1" max="1" width="19.81640625" customWidth="1"/>
     <col min="2" max="2" width="6.1796875" customWidth="1"/>
     <col min="3" max="4" width="11.453125" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -841,17 +624,17 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>3586</v>
+        <v>7554</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2">
         <f>C2</f>
-        <v>3586</v>
+        <v>7554</v>
       </c>
       <c r="F2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -860,15 +643,16 @@
       </c>
       <c r="E12">
         <f>SUM(E2:E10)</f>
-        <v>3586</v>
+        <v>7554</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B7B0F1E-C979-4C21-B312-FEEDB3E52407}">
   <dimension ref="A1:F12"/>
   <sheetViews>
@@ -939,7 +723,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E18CACF-38E0-4F05-9197-203383C8FC18}">
   <dimension ref="A1:F12"/>
   <sheetViews>
@@ -1010,7 +794,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65335C43-E3F8-4707-82AC-D64DB07E5F88}">
   <dimension ref="A1:F12"/>
   <sheetViews>
@@ -1080,7 +864,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F6CA172-7BA6-40DD-ABB6-E303E9E694A5}">
   <dimension ref="A1:F12"/>
   <sheetViews>
@@ -1151,7 +935,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1B96CF0-432F-4A3E-940D-86E08F6940C7}">
   <dimension ref="A1:F12"/>
   <sheetViews>
@@ -1298,11 +1082,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C39777F-CEF0-4425-930E-295AE7C473DC}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D8" sqref="C7:D8"/>
     </sheetView>
   </sheetViews>
@@ -1387,11 +1171,228 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{355DE0EA-5B2C-4635-84EE-7D1B81ED29C7}">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.1796875" customWidth="1"/>
+    <col min="5" max="5" width="9.453125" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <v>80</v>
+      </c>
+      <c r="D2">
+        <f>B2*C2</f>
+        <v>8000</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>160</v>
+      </c>
+      <c r="C3">
+        <v>50</v>
+      </c>
+      <c r="D3">
+        <f>B3*C3</f>
+        <v>8000</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3">
+        <f>D3/8000</f>
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <f>H2+1</f>
+        <v>50</v>
+      </c>
+      <c r="H3">
+        <f>G3+C3 -1</f>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>1600</v>
+      </c>
+      <c r="C4">
+        <v>30</v>
+      </c>
+      <c r="D4">
+        <f>B4*C4</f>
+        <v>48000</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4">
+        <v>7</v>
+      </c>
+      <c r="G4">
+        <f>H3+1</f>
+        <v>100</v>
+      </c>
+      <c r="H4">
+        <f>G4+C4 -1</f>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>3200</v>
+      </c>
+      <c r="C5">
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <f>B5*C5</f>
+        <v>64000</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5">
+        <v>9</v>
+      </c>
+      <c r="G5">
+        <f>H4+1</f>
+        <v>130</v>
+      </c>
+      <c r="H5">
+        <f>G5+C5 -1</f>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>8000</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <f>B6*C6</f>
+        <v>48000</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6">
+        <f>D6/8000</f>
+        <v>6</v>
+      </c>
+      <c r="G6">
+        <f>H5+1</f>
+        <v>150</v>
+      </c>
+      <c r="H6">
+        <f>G6+C6 - 1</f>
+        <v>155</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <f>SUM(B2:B8)</f>
+        <v>13060</v>
+      </c>
+      <c r="C9">
+        <f>SUM(C2:C6)</f>
+        <v>186</v>
+      </c>
+      <c r="D9">
+        <f>SUM(D2:D8)</f>
+        <v>176000</v>
+      </c>
+      <c r="F9">
+        <f>SUM(F2:F6)</f>
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8A806B9-8F96-4CFC-8F80-C6046C4BB66C}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
@@ -1720,7 +1721,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P33" sqref="P33"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1756,14 +1757,14 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D2">
         <v>256</v>
       </c>
       <c r="E2">
         <f t="shared" ref="E2" si="0">C2*D2</f>
-        <v>512</v>
+        <v>2048</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -1777,7 +1778,7 @@
       </c>
       <c r="E13">
         <f>SUM(E2:E11)</f>
-        <v>512</v>
+        <v>2048</v>
       </c>
     </row>
   </sheetData>
@@ -1787,7 +1788,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA754253-1AC6-4AC6-91AF-37AC71E22B02}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6700B15-078B-4B8C-B149-C046CE8CC3B4}">
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1830,14 +1831,14 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>7554</v>
+        <v>7663</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2">
         <f>C2</f>
-        <v>7554</v>
+        <v>7663</v>
       </c>
       <c r="F2" t="s">
         <v>38</v>
@@ -1849,12 +1850,11 @@
       </c>
       <c r="E12">
         <f>SUM(E2:E10)</f>
-        <v>7554</v>
+        <v>7663</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1987,77 +1987,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6700B15-078B-4B8C-B149-C046CE8CC3B4}">
-  <dimension ref="A1:F12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="19.81640625" customWidth="1"/>
-    <col min="2" max="2" width="6.1796875" customWidth="1"/>
-    <col min="3" max="4" width="11.453125" customWidth="1"/>
-    <col min="6" max="6" width="21.26953125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>7663</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <f>C2</f>
-        <v>7663</v>
-      </c>
-      <c r="F2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12">
-        <f>SUM(E2:E10)</f>
-        <v>7663</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{382A0DF3-A6E2-4E63-819F-0B238C4B218B}">
   <dimension ref="A1:F12"/>
   <sheetViews>
@@ -2152,7 +2081,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4FAB9BB-644E-4DE7-A6F3-2DB946584AF9}">
   <dimension ref="A1:F12"/>
   <sheetViews>
@@ -2223,7 +2152,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12C5024D-5883-452F-AA38-8CA5B65145D7}">
   <dimension ref="A1:F12"/>
   <sheetViews>
@@ -2294,7 +2223,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EE80BDF-E657-4A2B-B23B-E05D3D83C462}">
   <dimension ref="A1:F12"/>
   <sheetViews>
@@ -2365,7 +2294,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EED8C9F-5BE2-4E98-B5FC-EB226A731849}">
   <dimension ref="A1:F12"/>
   <sheetViews>
@@ -2436,7 +2365,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C669B32-4B46-4AD0-A79C-01B618483F1F}">
   <dimension ref="A1:F12"/>
   <sheetViews>
@@ -2524,4 +2453,75 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D02A195F-A94B-43B9-B272-B66DEB6E2820}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>3586</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f>C2</f>
+        <v>3586</v>
+      </c>
+      <c r="F2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <f>SUM(E2:E10)</f>
+        <v>3586</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Moved logics to 3E to fix corruption bug
</commit_message>
<xml_diff>
--- a/docs/allocation.xlsx
+++ b/docs/allocation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2CA0809-5E5F-423D-A120-6520C7B26FBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07999251-4104-4C90-BB0B-2B2A80DAE420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" firstSheet="7" activeTab="16" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" firstSheet="6" activeTab="18" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic (Bank 0x13 - 0x3A)" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="60">
   <si>
     <t>Type</t>
   </si>
@@ -221,6 +221,9 @@
   </si>
   <si>
     <t>logicEntryAddresses</t>
+  </si>
+  <si>
+    <t>pictureFile</t>
   </si>
 </sst>
 </file>
@@ -585,7 +588,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1391,8 +1394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8A806B9-8F96-4CFC-8F80-C6046C4BB66C}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1443,7 +1446,7 @@
         <v>16</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B9" si="0">B2+ E2+1</f>
+        <f>B2+ E2+1</f>
         <v>186</v>
       </c>
       <c r="C3">
@@ -1453,7 +1456,7 @@
         <v>255</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E6" si="1">C3*D3</f>
+        <f t="shared" ref="E3:E6" si="0">C3*D3</f>
         <v>1275</v>
       </c>
     </row>
@@ -1462,7 +1465,7 @@
         <v>17</v>
       </c>
       <c r="B4">
-        <f t="shared" si="0"/>
+        <f>B3+ E3+1</f>
         <v>1462</v>
       </c>
       <c r="C4">
@@ -1472,7 +1475,7 @@
         <v>255</v>
       </c>
       <c r="E4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1275</v>
       </c>
     </row>
@@ -1481,7 +1484,7 @@
         <v>18</v>
       </c>
       <c r="B5">
-        <f t="shared" si="0"/>
+        <f>B4+ E4+1</f>
         <v>2738</v>
       </c>
       <c r="C5">
@@ -1491,7 +1494,7 @@
         <v>255</v>
       </c>
       <c r="E5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1275</v>
       </c>
     </row>
@@ -1500,7 +1503,7 @@
         <v>19</v>
       </c>
       <c r="B6">
-        <f t="shared" si="0"/>
+        <f>B5+ E5+1</f>
         <v>4014</v>
       </c>
       <c r="C6">
@@ -1510,46 +1513,8 @@
         <v>255</v>
       </c>
       <c r="E6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1275</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7">
-        <f t="shared" si="0"/>
-        <v>5290</v>
-      </c>
-      <c r="C7">
-        <v>8</v>
-      </c>
-      <c r="D7">
-        <v>255</v>
-      </c>
-      <c r="E7">
-        <f t="shared" ref="E7" si="2">C7*D7</f>
-        <v>2040</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8">
-        <f t="shared" si="0"/>
-        <v>7331</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8">
-        <v>255</v>
-      </c>
-      <c r="E8">
-        <f t="shared" ref="E8" si="3">C8*D8</f>
-        <v>510</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -1557,8 +1522,8 @@
         <v>28</v>
       </c>
       <c r="B9">
-        <f t="shared" si="0"/>
-        <v>7842</v>
+        <f>BANK0x3E!B4+ BANK0x3E!E4+1</f>
+        <v>5874</v>
       </c>
       <c r="C9">
         <v>10</v>
@@ -1567,7 +1532,7 @@
         <v>20</v>
       </c>
       <c r="E9">
-        <f t="shared" ref="E9" si="4">C9*D9</f>
+        <f t="shared" ref="E9" si="1">C9*D9</f>
         <v>200</v>
       </c>
     </row>
@@ -1577,7 +1542,7 @@
       </c>
       <c r="E13">
         <f>SUM(E2:E11)</f>
-        <v>8035</v>
+        <v>5485</v>
       </c>
     </row>
   </sheetData>
@@ -1719,8 +1684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1ECB7A9-D68D-4611-9022-3CBE081861CE}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P33" sqref="P33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1750,20 +1715,58 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D2">
         <v>256</v>
       </c>
       <c r="E2">
         <f t="shared" ref="E2" si="0">C2*D2</f>
-        <v>512</v>
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <f>E2 + 1</f>
+        <v>1537</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>255</v>
+      </c>
+      <c r="E3">
+        <f>C3*D3</f>
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4">
+        <f>B3+ E3+1</f>
+        <v>3578</v>
+      </c>
+      <c r="C4">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>255</v>
+      </c>
+      <c r="E4">
+        <f>C4*D4</f>
+        <v>2295</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -1777,7 +1780,7 @@
       </c>
       <c r="E13">
         <f>SUM(E2:E11)</f>
-        <v>512</v>
+        <v>5871</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected missing information on memory management bank
</commit_message>
<xml_diff>
--- a/docs/allocation.xlsx
+++ b/docs/allocation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07999251-4104-4C90-BB0B-2B2A80DAE420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A7E52D-BC6C-4A7F-B510-67B9E6F3AABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" firstSheet="6" activeTab="18" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" firstSheet="6" activeTab="15" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic (Bank 0x13 - 0x3A)" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="62">
   <si>
     <t>Type</t>
   </si>
@@ -224,6 +224,12 @@
   </si>
   <si>
     <t>pictureFile</t>
+  </si>
+  <si>
+    <t>allocationArray</t>
+  </si>
+  <si>
+    <t>Allocation Segment</t>
   </si>
 </sst>
 </file>
@@ -588,7 +594,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1305,8 +1311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C39777F-CEF0-4425-930E-295AE7C473DC}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="C7:D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1360,19 +1366,45 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3">
+        <f>B4-E3</f>
+        <v>7971</v>
+      </c>
+      <c r="C3">
+        <v>186</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <f>C3*D3</f>
+        <v>186</v>
+      </c>
+      <c r="F3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>56</v>
       </c>
-      <c r="B3">
-        <v>8156</v>
-      </c>
-      <c r="C3">
+      <c r="B4">
+        <f>8192-E4</f>
+        <v>8157</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <f>C4*D4</f>
         <v>35</v>
       </c>
-      <c r="E3">
-        <f>C3</f>
-        <v>35</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="F4" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1382,7 +1414,7 @@
       </c>
       <c r="E12">
         <f>SUM(E2:E10)</f>
-        <v>1621</v>
+        <v>1807</v>
       </c>
     </row>
   </sheetData>
@@ -1684,7 +1716,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1ECB7A9-D68D-4611-9022-3CBE081861CE}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Corrected incorrect banks configured in dynamic memory
</commit_message>
<xml_diff>
--- a/docs/allocation.xlsx
+++ b/docs/allocation.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A7E52D-BC6C-4A7F-B510-67B9E6F3AABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B102954E-4619-4F39-9E8E-AA0E54920AE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" firstSheet="6" activeTab="15" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Dynamic (Bank 0x13 - 0x3A)" sheetId="2" r:id="rId1"/>
+    <sheet name="Dynamic (Bank 0x13 - 0x28)" sheetId="2" r:id="rId1"/>
     <sheet name="Bank0x1" sheetId="6" r:id="rId2"/>
     <sheet name="Bank0x2" sheetId="7" r:id="rId3"/>
     <sheet name="Bank0x3" sheetId="3" r:id="rId4"/>
@@ -193,15 +193,6 @@
     <t>MEKA Main Logic and execute logic</t>
   </si>
   <si>
-    <t>0x35-0x3A</t>
-  </si>
-  <si>
-    <t>0x2C-0x34</t>
-  </si>
-  <si>
-    <t>0x15-0x2B</t>
-  </si>
-  <si>
     <t>0x14</t>
   </si>
   <si>
@@ -230,6 +221,15 @@
   </si>
   <si>
     <t>Allocation Segment</t>
+  </si>
+  <si>
+    <t>0x15-0x1A</t>
+  </si>
+  <si>
+    <t>0x1B-0x22</t>
+  </si>
+  <si>
+    <t>0x23-0x28</t>
   </si>
 </sst>
 </file>
@@ -593,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{355DE0EA-5B2C-4635-84EE-7D1B81ED29C7}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -649,7 +649,7 @@
         <v>8000</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -676,7 +676,7 @@
         <v>8000</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F3">
         <f>D3/8000</f>
@@ -706,10 +706,10 @@
         <v>48000</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="F4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G4">
         <f>H3+1</f>
@@ -735,10 +735,10 @@
         <v>64000</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="F5">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G5">
         <f>H4+1</f>
@@ -764,7 +764,7 @@
         <v>48000</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="F6">
         <f>D6/8000</f>
@@ -797,7 +797,7 @@
       </c>
       <c r="F9">
         <f>SUM(F2:F6)</f>
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1311,7 +1311,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C39777F-CEF0-4425-930E-295AE7C473DC}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1361,12 +1361,12 @@
         <v>1586</v>
       </c>
       <c r="F2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B3">
         <f>B4-E3</f>
@@ -1383,12 +1383,12 @@
         <v>186</v>
       </c>
       <c r="F3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B4">
         <f>8192-E4</f>
@@ -1405,7 +1405,7 @@
         <v>35</v>
       </c>
       <c r="F4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1694,7 +1694,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -1747,7 +1747,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1803,7 +1803,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -2530,7 +2530,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B11">
         <f>8191-E11</f>

</xml_diff>

<commit_message>
Removed two banks from medium to make space for division tables
</commit_message>
<xml_diff>
--- a/docs/allocation.xlsx
+++ b/docs/allocation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2775C98F-6F7B-41B9-8E44-3D99ADE7D7C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC9F1448-FAD3-456D-B84B-EC95EA03FF22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" firstSheet="2" activeTab="15" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic (Bank 0x13 - 0x28)" sheetId="2" r:id="rId1"/>
@@ -215,12 +215,6 @@
     <t>0x15-0x1A</t>
   </si>
   <si>
-    <t>0x1B-0x22</t>
-  </si>
-  <si>
-    <t>0x23-0x28</t>
-  </si>
-  <si>
     <t>Init code meka driver</t>
   </si>
   <si>
@@ -231,6 +225,12 @@
   </si>
   <si>
     <t xml:space="preserve">   </t>
+  </si>
+  <si>
+    <t>0x1B-0x20</t>
+  </si>
+  <si>
+    <t>0x21-0x26</t>
   </si>
 </sst>
 </file>
@@ -594,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{355DE0EA-5B2C-4635-84EE-7D1B81ED29C7}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -729,17 +729,17 @@
         <v>3200</v>
       </c>
       <c r="C5">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D5">
         <f>B5*C5</f>
-        <v>64000</v>
+        <v>48000</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="F5">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G5">
         <f>H4+1</f>
@@ -747,7 +747,7 @@
       </c>
       <c r="H5">
         <f>G5+C5 -1</f>
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -765,7 +765,7 @@
         <v>48000</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="F6">
         <f>D6/8000</f>
@@ -773,11 +773,11 @@
       </c>
       <c r="G6">
         <f>H5+1</f>
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="H6">
         <f>G6+C6 - 1</f>
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -790,15 +790,15 @@
       </c>
       <c r="C9">
         <f>SUM(C2:C6)</f>
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="D9">
         <f>SUM(D2:D8)</f>
-        <v>176000</v>
+        <v>160000</v>
       </c>
       <c r="F9">
         <f>SUM(F2:F6)</f>
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1312,7 +1312,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{470FF23A-2CF2-4342-A127-6A0CAC1D7ECC}">
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
@@ -1376,7 +1376,7 @@
     </row>
     <row r="34" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M34" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -2459,7 +2459,7 @@
         <v>8191</v>
       </c>
       <c r="F2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -2530,7 +2530,7 @@
         <v>8191</v>
       </c>
       <c r="F2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -2601,7 +2601,7 @@
         <v>8191</v>
       </c>
       <c r="F2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Memory address errors corrected
</commit_message>
<xml_diff>
--- a/docs/allocation.xlsx
+++ b/docs/allocation.xlsx
@@ -8,32 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC9F1448-FAD3-456D-B84B-EC95EA03FF22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAFB6AAD-FDF9-413E-B03D-56CAAB4DDD88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" firstSheet="6" activeTab="19" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Dynamic (Bank 0x13 - 0x28)" sheetId="2" r:id="rId1"/>
-    <sheet name="Bank0x1" sheetId="6" r:id="rId2"/>
-    <sheet name="Bank0x2" sheetId="7" r:id="rId3"/>
-    <sheet name="Bank0x3" sheetId="3" r:id="rId4"/>
-    <sheet name="Bank0x4" sheetId="8" r:id="rId5"/>
-    <sheet name="Bank0x5" sheetId="9" r:id="rId6"/>
-    <sheet name="Bank0x6" sheetId="10" r:id="rId7"/>
-    <sheet name="Bank0x7" sheetId="11" r:id="rId8"/>
-    <sheet name="Bank0x8" sheetId="12" r:id="rId9"/>
-    <sheet name="Bank0x9" sheetId="13" r:id="rId10"/>
-    <sheet name="Bank0xA" sheetId="14" r:id="rId11"/>
-    <sheet name="Bank0xB" sheetId="15" r:id="rId12"/>
-    <sheet name="Bank0xC" sheetId="16" r:id="rId13"/>
-    <sheet name="Bank0xD" sheetId="17" r:id="rId14"/>
-    <sheet name="Bank0xE" sheetId="18" r:id="rId15"/>
-    <sheet name="Bank0xF" sheetId="21" r:id="rId16"/>
-    <sheet name="Bank0x10" sheetId="19" r:id="rId17"/>
-    <sheet name="BANK0x3C" sheetId="1" r:id="rId18"/>
-    <sheet name="BANK0x3D" sheetId="5" r:id="rId19"/>
-    <sheet name="BANK0x3E" sheetId="20" r:id="rId20"/>
-    <sheet name="Golden" sheetId="4" r:id="rId21"/>
+    <sheet name="Dynamic (Bank 0x13 - 0x26)" sheetId="2" r:id="rId1"/>
+    <sheet name="Flood Banks (Bank 0x27 - 0x30)" sheetId="22" r:id="rId2"/>
+    <sheet name="Div Banks (Bank 0x31 - 0x3A)" sheetId="23" r:id="rId3"/>
+    <sheet name="Bank0x1" sheetId="6" r:id="rId4"/>
+    <sheet name="Bank0x2" sheetId="7" r:id="rId5"/>
+    <sheet name="Bank0x3" sheetId="3" r:id="rId6"/>
+    <sheet name="Bank0x4" sheetId="8" r:id="rId7"/>
+    <sheet name="Bank0x5" sheetId="9" r:id="rId8"/>
+    <sheet name="Bank0x6" sheetId="10" r:id="rId9"/>
+    <sheet name="Bank0x7" sheetId="11" r:id="rId10"/>
+    <sheet name="Bank0x8" sheetId="12" r:id="rId11"/>
+    <sheet name="Bank0x9" sheetId="13" r:id="rId12"/>
+    <sheet name="Bank0xA" sheetId="14" r:id="rId13"/>
+    <sheet name="Bank0xB" sheetId="15" r:id="rId14"/>
+    <sheet name="Bank0xC" sheetId="16" r:id="rId15"/>
+    <sheet name="Bank0xD" sheetId="17" r:id="rId16"/>
+    <sheet name="Bank0xE" sheetId="18" r:id="rId17"/>
+    <sheet name="Bank0xF" sheetId="21" r:id="rId18"/>
+    <sheet name="Bank0x10" sheetId="19" r:id="rId19"/>
+    <sheet name="Bank0x11" sheetId="24" r:id="rId20"/>
+    <sheet name="BANK0x3C" sheetId="1" r:id="rId21"/>
+    <sheet name="BANK0x3D" sheetId="5" r:id="rId22"/>
+    <sheet name="BANK0x3E" sheetId="20" r:id="rId23"/>
+    <sheet name="Golden" sheetId="4" r:id="rId24"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="66">
   <si>
     <t>Type</t>
   </si>
@@ -231,6 +234,18 @@
   </si>
   <si>
     <t>0x21-0x26</t>
+  </si>
+  <si>
+    <t>Mult Table</t>
+  </si>
+  <si>
+    <t>Flood Queue</t>
+  </si>
+  <si>
+    <t>Division Tables</t>
+  </si>
+  <si>
+    <t>Identical For Every Bank. Holds precomputed division results to 4 decimal places. Bank 3B holds division table metadata</t>
   </si>
 </sst>
 </file>
@@ -594,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{355DE0EA-5B2C-4635-84EE-7D1B81ED29C7}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -808,6 +823,148 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EED8C9F-5BE2-4E98-B5FC-EB226A731849}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="30.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>8191</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f>C2</f>
+        <v>8191</v>
+      </c>
+      <c r="F2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <f>SUM(E2:E10)</f>
+        <v>8191</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C669B32-4B46-4AD0-A79C-01B618483F1F}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="17.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>8191</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f>C2</f>
+        <v>8191</v>
+      </c>
+      <c r="F2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <f>SUM(E2:E10)</f>
+        <v>8191</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D02A195F-A94B-43B9-B272-B66DEB6E2820}">
   <dimension ref="A1:F12"/>
   <sheetViews>
@@ -878,7 +1035,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B7B0F1E-C979-4C21-B312-FEEDB3E52407}">
   <dimension ref="A1:F12"/>
   <sheetViews>
@@ -949,7 +1106,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E18CACF-38E0-4F05-9197-203383C8FC18}">
   <dimension ref="A1:F12"/>
   <sheetViews>
@@ -1020,7 +1177,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65335C43-E3F8-4707-82AC-D64DB07E5F88}">
   <dimension ref="A1:F12"/>
   <sheetViews>
@@ -1090,7 +1247,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F6CA172-7BA6-40DD-ABB6-E303E9E694A5}">
   <dimension ref="A1:F12"/>
   <sheetViews>
@@ -1161,7 +1318,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1B96CF0-432F-4A3E-940D-86E08F6940C7}">
   <dimension ref="A1:F12"/>
   <sheetViews>
@@ -1308,7 +1465,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{470FF23A-2CF2-4342-A127-6A0CAC1D7ECC}">
   <dimension ref="A1:M34"/>
   <sheetViews>
@@ -1384,12 +1541,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C39777F-CEF0-4425-930E-295AE7C473DC}">
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1499,7 +1656,199 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C481C6A-559C-4191-936B-FDDAE6C4B3A5}">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>2128</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f>C2</f>
+        <v>2128</v>
+      </c>
+      <c r="F2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3">
+        <f>C2</f>
+        <v>2128</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>5728</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4">
+        <f>B3+E3+1</f>
+        <v>7857</v>
+      </c>
+      <c r="C4">
+        <v>336</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <f>C4 * D4</f>
+        <v>336</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E10">
+        <f>SUM(E2:E8)</f>
+        <v>8192</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84FE8641-C02D-4ECA-9797-EDC79FC57C57}">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>7856</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f>C2</f>
+        <v>7856</v>
+      </c>
+      <c r="F2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3">
+        <f>E2</f>
+        <v>7856</v>
+      </c>
+      <c r="C3">
+        <v>336</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <f>C3 * D3</f>
+        <v>336</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E9">
+        <f>SUM(E2:E7)</f>
+        <v>8192</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8A806B9-8F96-4CFC-8F80-C6046C4BB66C}">
   <dimension ref="A1:F13"/>
   <sheetViews>
@@ -1660,12 +2009,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A86A6CAE-A2FB-4700-AF3B-F451BF94FBFE}">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N33" sqref="N33"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1789,7 +2138,320 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1ECB7A9-D68D-4611-9022-3CBE081861CE}">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>256</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ref="E2" si="0">C2*D2</f>
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <f>E2 + 1</f>
+        <v>1537</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>255</v>
+      </c>
+      <c r="E3">
+        <f>C3*D3</f>
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4">
+        <f>B3+ E3+1</f>
+        <v>3578</v>
+      </c>
+      <c r="C4">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>255</v>
+      </c>
+      <c r="E4">
+        <f>C4*D4</f>
+        <v>2295</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <f>SUM(E2:E11)</f>
+        <v>5871</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF57E188-51E7-49EE-9F4F-07D9A5354CD1}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="22.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>256</v>
+      </c>
+      <c r="E2">
+        <f>C2*D2</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3">
+        <f>B2+ E2+1</f>
+        <v>257</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>256</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3" si="0">C3*D3</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4">
+        <f>B3+ E3+1</f>
+        <v>514</v>
+      </c>
+      <c r="C4">
+        <v>500</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4" si="1">C4*D4</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5">
+        <f>B4+ E4+1</f>
+        <v>1015</v>
+      </c>
+      <c r="C5">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ref="E5" si="2">C5*D5</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10">
+        <f>SUM(E2:E9)</f>
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11">
+        <v>1023</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{241BE7AF-6CB8-422B-A8C0-1FDCC7BE361F}">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="100.453125" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>8191</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f>C2</f>
+        <v>8191</v>
+      </c>
+      <c r="F2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <f>SUM(E2:E8)</f>
+        <v>8191</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA754253-1AC6-4AC6-91AF-37AC71E22B02}">
   <dimension ref="A1:F12"/>
   <sheetViews>
@@ -1861,244 +2523,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1ECB7A9-D68D-4611-9022-3CBE081861CE}">
-  <dimension ref="A1:F13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="19.81640625" customWidth="1"/>
-    <col min="2" max="2" width="6.1796875" customWidth="1"/>
-    <col min="3" max="4" width="11.453125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>6</v>
-      </c>
-      <c r="D2">
-        <v>256</v>
-      </c>
-      <c r="E2">
-        <f t="shared" ref="E2" si="0">C2*D2</f>
-        <v>1536</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3">
-        <f>E2 + 1</f>
-        <v>1537</v>
-      </c>
-      <c r="C3">
-        <v>8</v>
-      </c>
-      <c r="D3">
-        <v>255</v>
-      </c>
-      <c r="E3">
-        <f>C3*D3</f>
-        <v>2040</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4">
-        <f>B3+ E3+1</f>
-        <v>3578</v>
-      </c>
-      <c r="C4">
-        <v>9</v>
-      </c>
-      <c r="D4">
-        <v>255</v>
-      </c>
-      <c r="E4">
-        <f>C4*D4</f>
-        <v>2295</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13">
-        <f>SUM(E2:E11)</f>
-        <v>5871</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF57E188-51E7-49EE-9F4F-07D9A5354CD1}">
-  <dimension ref="A1:E11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="22.7265625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>256</v>
-      </c>
-      <c r="E2">
-        <f>C2*D2</f>
-        <v>256</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3">
-        <f>B2+ E2+1</f>
-        <v>257</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>256</v>
-      </c>
-      <c r="E3">
-        <f t="shared" ref="E3" si="0">C3*D3</f>
-        <v>256</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4">
-        <f>B3+ E3+1</f>
-        <v>514</v>
-      </c>
-      <c r="C4">
-        <v>500</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <f t="shared" ref="E4" si="1">C4*D4</f>
-        <v>500</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5">
-        <f>B4+ E4+1</f>
-        <v>1015</v>
-      </c>
-      <c r="C5">
-        <v>11</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <f t="shared" ref="E5" si="2">C5*D5</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10">
-        <f>SUM(E2:E9)</f>
-        <v>1023</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11">
-        <v>1023</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6700B15-078B-4B8C-B149-C046CE8CC3B4}">
   <dimension ref="A1:F12"/>
   <sheetViews>
@@ -2169,7 +2594,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{382A0DF3-A6E2-4E63-819F-0B238C4B218B}">
   <dimension ref="A1:F12"/>
   <sheetViews>
@@ -2264,7 +2689,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4FAB9BB-644E-4DE7-A6F3-2DB946584AF9}">
   <dimension ref="A1:F12"/>
   <sheetViews>
@@ -2335,7 +2760,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12C5024D-5883-452F-AA38-8CA5B65145D7}">
   <dimension ref="A1:F12"/>
   <sheetViews>
@@ -2406,7 +2831,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EE80BDF-E657-4A2B-B23B-E05D3D83C462}">
   <dimension ref="A1:F12"/>
   <sheetViews>
@@ -2474,146 +2899,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EED8C9F-5BE2-4E98-B5FC-EB226A731849}">
-  <dimension ref="A1:F12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="19.81640625" customWidth="1"/>
-    <col min="2" max="2" width="6.1796875" customWidth="1"/>
-    <col min="3" max="4" width="11.453125" customWidth="1"/>
-    <col min="6" max="6" width="30.1796875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>8191</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <f>C2</f>
-        <v>8191</v>
-      </c>
-      <c r="F2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12">
-        <f>SUM(E2:E10)</f>
-        <v>8191</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C669B32-4B46-4AD0-A79C-01B618483F1F}">
-  <dimension ref="A1:F12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="19.81640625" customWidth="1"/>
-    <col min="2" max="2" width="6.1796875" customWidth="1"/>
-    <col min="3" max="4" width="11.453125" customWidth="1"/>
-    <col min="6" max="6" width="17.90625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>8191</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <f>C2</f>
-        <v>8191</v>
-      </c>
-      <c r="F2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12">
-        <f>SUM(E2:E10)</f>
-        <v>8191</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Placing tables into memory
</commit_message>
<xml_diff>
--- a/docs/allocation.xlsx
+++ b/docs/allocation.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAFB6AAD-FDF9-413E-B03D-56CAAB4DDD88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A103E720-8323-43A1-97D3-03AB67060E9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" firstSheet="6" activeTab="19" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" activeTab="2" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic (Bank 0x13 - 0x26)" sheetId="2" r:id="rId1"/>
     <sheet name="Flood Banks (Bank 0x27 - 0x30)" sheetId="22" r:id="rId2"/>
-    <sheet name="Div Banks (Bank 0x31 - 0x3A)" sheetId="23" r:id="rId3"/>
+    <sheet name="Div Banks (Bank 0x31 - 0x3B)" sheetId="23" r:id="rId3"/>
     <sheet name="Bank0x1" sheetId="6" r:id="rId4"/>
     <sheet name="Bank0x2" sheetId="7" r:id="rId5"/>
     <sheet name="Bank0x3" sheetId="3" r:id="rId6"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="71">
   <si>
     <t>Type</t>
   </si>
@@ -245,7 +245,30 @@
     <t>Division Tables</t>
   </si>
   <si>
-    <t>Identical For Every Bank. Holds precomputed division results to 4 decimal places. Bank 3B holds division table metadata</t>
+    <t>These banks hold precomputed division results to 4 decimal places. 
+It supports numerators from 1 to 167 and denominators from 2 to 167
+The first result is 1 / 2 followed by 1 / 3 . . . 1 / 167 followed by 2 / 2  and so on. 
+No numerator group overlaps into another bank
+Denominators of 0 and 1 are skipped for obvious reasons
+The results are in little endian format with the mantissa portion stored as an integer
+The metadata for the tables are only stored on bank 0x31
+ There are two forms of metadata a bank table listing which indicates which bank a numerator group is stored on. It a simple one byte list, with the first one being for numerator group 1.
+The address metadata indicates at which address each numerator group starts with. It is stored in little endian two byte format, with the first address being for numerator 1.</t>
+  </si>
+  <si>
+    <t>Bank Metadata (31 only)</t>
+  </si>
+  <si>
+    <t>Address Metadata</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>These numbers are out and need fixing. May be code rather than Excel</t>
+  </si>
+  <si>
+    <t>Ends</t>
   </si>
 </sst>
 </file>
@@ -289,10 +312,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1765,7 +1791,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84FE8641-C02D-4ECA-9797-EDC79FC57C57}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -2249,18 +2275,19 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF57E188-51E7-49EE-9F4F-07D9A5354CD1}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="60.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -2276,8 +2303,11 @@
       <c r="E1" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -2294,8 +2324,12 @@
         <f>C2*D2</f>
         <v>256</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F2" t="str">
+        <f>DEC2HEX(HEX2DEC("400"))</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -2313,8 +2347,12 @@
         <f t="shared" ref="E3" si="0">C3*D3</f>
         <v>256</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F3" t="str">
+        <f>DEC2HEX(HEX2DEC(F2) + E2)</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -2332,8 +2370,12 @@
         <f t="shared" ref="E4" si="1">C4*D4</f>
         <v>500</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F4" t="str">
+        <f>DEC2HEX(HEX2DEC(F3) + E3)</f>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -2351,8 +2393,17 @@
         <f t="shared" ref="E5" si="2">C5*D5</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F5" t="str">
+        <f>DEC2HEX(HEX2DEC(F4) + E4)</f>
+        <v>7F4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -2361,7 +2412,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -2377,21 +2428,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{241BE7AF-6CB8-422B-A8C0-1FDCC7BE361F}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="100.453125" customWidth="1"/>
+    <col min="1" max="1" width="56.81640625" customWidth="1"/>
     <col min="2" max="2" width="6.1796875" customWidth="1"/>
     <col min="3" max="4" width="11.453125" customWidth="1"/>
     <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -2410,44 +2462,119 @@
       <c r="F1" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>8191</v>
+        <v>7470</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2">
         <f>C2</f>
-        <v>8191</v>
+        <v>7470</v>
       </c>
       <c r="F2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="G2" t="str">
+        <f>DEC2HEX(HEX2DEC("A000"))</f>
+        <v>A000</v>
+      </c>
+      <c r="H2" t="str">
+        <f t="shared" ref="H2:H3" si="0">DEC2HEX(HEX2DEC(G2)+E2-1)</f>
+        <v>BD2D</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3">
+        <f>C2</f>
+        <v>7470</v>
+      </c>
+      <c r="C3">
+        <v>167</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <f>C3</f>
+        <v>167</v>
+      </c>
+      <c r="G3" t="str">
+        <f>DEC2HEX(HEX2DEC(G2) + E2)</f>
+        <v>BD2E</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" si="0"/>
+        <v>BDD4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4">
+        <f>B3+E3</f>
+        <v>7637</v>
+      </c>
+      <c r="C4">
+        <v>334</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>334</v>
+      </c>
+      <c r="G4" t="str">
+        <f>DEC2HEX(HEX2DEC(G3) + E3)</f>
+        <v>BDD5</v>
+      </c>
+      <c r="H4" t="str">
+        <f>DEC2HEX(HEX2DEC(G4)+E4-1)</f>
+        <v>BF22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E5">
+        <f>SUM(E2+E4)</f>
+        <v>7804</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:8" ht="253" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E10">
         <f>SUM(E2:E8)</f>
-        <v>8191</v>
+        <v>15775</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
First cut of division
</commit_message>
<xml_diff>
--- a/docs/allocation.xlsx
+++ b/docs/allocation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A103E720-8323-43A1-97D3-03AB67060E9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEDC09E3-3450-4987-9026-2C86A4D82D55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" activeTab="2" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
@@ -2431,7 +2431,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Fixed wrong calculation for large division error
</commit_message>
<xml_diff>
--- a/docs/allocation.xlsx
+++ b/docs/allocation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEDC09E3-3450-4987-9026-2C86A4D82D55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF5DFC76-6FF1-4BBC-AC57-23385A67C5AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" activeTab="2" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
@@ -2431,7 +2431,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Fixed weird dotting issue caused by corrupted multiplation table
</commit_message>
<xml_diff>
--- a/docs/allocation.xlsx
+++ b/docs/allocation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ABBC046-EC5B-4FCA-9980-C7807A3C5E5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF665D41-3117-47B0-8456-4EB2ECB37BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="14" activeTab="20" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic (Bank 0x13 - 0x26)" sheetId="2" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="74">
   <si>
     <t>Type</t>
   </si>
@@ -1659,8 +1659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C481C6A-559C-4191-936B-FDDAE6C4B3A5}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1719,9 +1719,6 @@
       <c r="E2">
         <f>C2*D2</f>
         <v>2128</v>
-      </c>
-      <c r="F2" t="s">
-        <v>48</v>
       </c>
       <c r="G2">
         <f>B2+C2-1</f>
@@ -1928,8 +1925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84FE8641-C02D-4ECA-9797-EDC79FC57C57}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1976,9 +1973,6 @@
       <c r="E2">
         <f>C2</f>
         <v>7856</v>
-      </c>
-      <c r="F2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Now loading charset into memory
</commit_message>
<xml_diff>
--- a/docs/allocation.xlsx
+++ b/docs/allocation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3CA353E-9C35-41ED-B924-154167E347EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{067080AF-DE01-458E-B3A8-A58A1AAAE66C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" firstSheet="12" activeTab="25" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
@@ -2622,7 +2622,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2663,7 +2663,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="str">
-        <f>DEC2HEX(HEX2DEC(D2)+C2-1)</f>
+        <f t="shared" ref="E2:E7" si="0">DEC2HEX(HEX2DEC(D2)+C2-1)</f>
         <v>95FF</v>
       </c>
     </row>
@@ -2683,7 +2683,7 @@
         <v>9600</v>
       </c>
       <c r="E3" t="str">
-        <f>DEC2HEX(HEX2DEC(D3)+C3-1)</f>
+        <f t="shared" si="0"/>
         <v>CA2F</v>
       </c>
     </row>
@@ -2703,7 +2703,7 @@
         <v>CA30</v>
       </c>
       <c r="E4" t="str">
-        <f>DEC2HEX(HEX2DEC(D4)+C4-1)</f>
+        <f t="shared" si="0"/>
         <v>CFFF</v>
       </c>
     </row>
@@ -2716,15 +2716,15 @@
         <v>53248</v>
       </c>
       <c r="C5">
-        <v>316</v>
+        <v>1264</v>
       </c>
       <c r="D5" t="str">
         <f>DEC2HEX(B4 + C4)</f>
         <v>D000</v>
       </c>
       <c r="E5" t="str">
-        <f>DEC2HEX(HEX2DEC(D5)+C5-1)</f>
-        <v>D13B</v>
+        <f t="shared" si="0"/>
+        <v>D4EF</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -2733,18 +2733,18 @@
       </c>
       <c r="B6">
         <f>B5+C5</f>
-        <v>53564</v>
+        <v>54512</v>
       </c>
       <c r="C6">
-        <v>196</v>
+        <v>784</v>
       </c>
       <c r="D6" t="str">
         <f>DEC2HEX(B5 + C5)</f>
-        <v>D13C</v>
+        <v>D4F0</v>
       </c>
       <c r="E6" t="str">
-        <f>DEC2HEX(HEX2DEC(D6)+C6-1)</f>
-        <v>D1FF</v>
+        <f t="shared" si="0"/>
+        <v>D7FF</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -2753,18 +2753,18 @@
       </c>
       <c r="B7">
         <f>B6+C6</f>
-        <v>53760</v>
+        <v>55296</v>
       </c>
       <c r="C7">
         <v>2400</v>
       </c>
       <c r="D7" t="str">
         <f>DEC2HEX(B6 + C6)</f>
-        <v>D200</v>
+        <v>D800</v>
       </c>
       <c r="E7" t="str">
-        <f>DEC2HEX(HEX2DEC(D7)+C7-1)</f>
-        <v>DB5F</v>
+        <f t="shared" si="0"/>
+        <v>E15F</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -2773,7 +2773,7 @@
       </c>
       <c r="C13">
         <f>SUM(C2:C7)</f>
-        <v>56160</v>
+        <v>57696</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -2790,7 +2790,7 @@
       </c>
       <c r="C15">
         <f>C14-C13</f>
-        <v>73311</v>
+        <v>71775</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Now loading entire ISO charset
</commit_message>
<xml_diff>
--- a/docs/allocation.xlsx
+++ b/docs/allocation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{067080AF-DE01-458E-B3A8-A58A1AAAE66C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2580BC96-2AD2-47FF-A151-F3FFB8F746A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" firstSheet="12" activeTab="25" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="82">
   <si>
     <t>Type</t>
   </si>
@@ -2619,10 +2619,10 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADD84C88-ECC4-4FFE-AD9A-78DE6241FE29}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2663,7 +2663,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="str">
-        <f t="shared" ref="E2:E7" si="0">DEC2HEX(HEX2DEC(D2)+C2-1)</f>
+        <f t="shared" ref="E2:E6" si="0">DEC2HEX(HEX2DEC(D2)+C2-1)</f>
         <v>95FF</v>
       </c>
     </row>
@@ -2716,7 +2716,7 @@
         <v>53248</v>
       </c>
       <c r="C5">
-        <v>1264</v>
+        <v>2560</v>
       </c>
       <c r="D5" t="str">
         <f>DEC2HEX(B4 + C4)</f>
@@ -2724,73 +2724,53 @@
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
-        <v>D4EF</v>
+        <v>D9FF</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="B6">
         <f>B5+C5</f>
-        <v>54512</v>
+        <v>55808</v>
       </c>
       <c r="C6">
-        <v>784</v>
+        <v>2561</v>
       </c>
       <c r="D6" t="str">
         <f>DEC2HEX(B5 + C5)</f>
-        <v>D4F0</v>
+        <v>DA00</v>
       </c>
       <c r="E6" t="str">
-        <f t="shared" si="0"/>
-        <v>D7FF</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B7">
-        <f>B6+C6</f>
-        <v>55296</v>
-      </c>
-      <c r="C7">
-        <v>2400</v>
-      </c>
-      <c r="D7" t="str">
-        <f>DEC2HEX(B6 + C6)</f>
-        <v>D800</v>
-      </c>
-      <c r="E7" t="str">
-        <f t="shared" si="0"/>
-        <v>E15F</v>
+        <f t="shared" ref="E6" si="1">DEC2HEX(HEX2DEC(D6)+C6-1)</f>
+        <v>E400</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12">
+        <f>SUM(C2:C6)</f>
+        <v>58369</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C13">
-        <f>SUM(C2:C7)</f>
-        <v>57696</v>
+        <v>129471</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C14">
-        <v>129471</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B15" t="s">
-        <v>77</v>
-      </c>
-      <c r="C15">
-        <f>C14-C13</f>
-        <v>71775</v>
+        <f>C13-C12</f>
+        <v>71102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Allocating space on banked ram for charset
</commit_message>
<xml_diff>
--- a/docs/allocation.xlsx
+++ b/docs/allocation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2580BC96-2AD2-47FF-A151-F3FFB8F746A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{180CF07A-724A-4AD8-B9C2-2F190B081CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" firstSheet="12" activeTab="25" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" activeTab="25" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic (Bank 0x13 - 0x26)" sheetId="2" r:id="rId1"/>
@@ -2622,7 +2622,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2663,7 +2663,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="str">
-        <f t="shared" ref="E2:E6" si="0">DEC2HEX(HEX2DEC(D2)+C2-1)</f>
+        <f t="shared" ref="E2:E5" si="0">DEC2HEX(HEX2DEC(D2)+C2-1)</f>
         <v>95FF</v>
       </c>
     </row>

</xml_diff>

<commit_message>
On PictureInstructionsVera: Adding files which were renamed so that CC65 doesn't delete them to project Allocation Work
</commit_message>
<xml_diff>
--- a/docs/allocation.xlsx
+++ b/docs/allocation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23668D2A-233E-45B9-8A86-ACA5E8D7D776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{114C7692-8438-45FE-9B4E-7596E6C3E396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="14" activeTab="20" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" firstSheet="14" activeTab="25" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic (Bank 0x13 - 0x26)" sheetId="2" r:id="rId1"/>
@@ -38,6 +38,7 @@
     <sheet name="BANK0x3D" sheetId="5" r:id="rId23"/>
     <sheet name="BANK0x3E" sheetId="20" r:id="rId24"/>
     <sheet name="Golden" sheetId="4" r:id="rId25"/>
+    <sheet name="Vera" sheetId="27" r:id="rId26"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="84">
   <si>
     <t>Type</t>
   </si>
@@ -287,6 +288,36 @@
   </si>
   <si>
     <t>Start Banked RAM Location Hex</t>
+  </si>
+  <si>
+    <t>Vera Address</t>
+  </si>
+  <si>
+    <t>Background Images</t>
+  </si>
+  <si>
+    <t>Priority Screen</t>
+  </si>
+  <si>
+    <t>Tilebase</t>
+  </si>
+  <si>
+    <t>Map Base</t>
+  </si>
+  <si>
+    <t>Total Used</t>
+  </si>
+  <si>
+    <t>Total Available</t>
+  </si>
+  <si>
+    <t>Remaining</t>
+  </si>
+  <si>
+    <t>Sprites</t>
+  </si>
+  <si>
+    <t>Volatile Buffer</t>
   </si>
 </sst>
 </file>
@@ -657,17 +688,17 @@
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.21875" customWidth="1"/>
-    <col min="5" max="5" width="9.44140625" customWidth="1"/>
+    <col min="1" max="1" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.1796875" customWidth="1"/>
+    <col min="5" max="5" width="9.453125" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -694,7 +725,7 @@
       </c>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -721,7 +752,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -751,7 +782,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -780,7 +811,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -809,7 +840,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -839,7 +870,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
@@ -874,15 +905,15 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
-    <col min="2" max="2" width="6.21875" customWidth="1"/>
-    <col min="3" max="4" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="24.77734375" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="24.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -902,7 +933,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -922,7 +953,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -944,15 +975,15 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
-    <col min="2" max="2" width="6.21875" customWidth="1"/>
-    <col min="3" max="4" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="30.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="30.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -972,7 +1003,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -993,7 +1024,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -1015,15 +1046,15 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
-    <col min="2" max="2" width="6.21875" customWidth="1"/>
-    <col min="3" max="4" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="17.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1043,7 +1074,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -1064,7 +1095,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -1086,15 +1117,15 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
-    <col min="2" max="2" width="6.21875" customWidth="1"/>
-    <col min="3" max="4" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1114,7 +1145,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -1135,7 +1166,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -1157,15 +1188,15 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
-    <col min="2" max="2" width="6.21875" customWidth="1"/>
-    <col min="3" max="4" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1185,7 +1216,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -1206,7 +1237,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -1228,15 +1259,15 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
-    <col min="2" max="2" width="6.21875" customWidth="1"/>
-    <col min="3" max="4" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1256,7 +1287,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -1277,7 +1308,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -1299,15 +1330,15 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
-    <col min="2" max="2" width="6.21875" customWidth="1"/>
-    <col min="3" max="4" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1327,7 +1358,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -1347,7 +1378,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -1369,15 +1400,15 @@
       <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
-    <col min="2" max="2" width="6.21875" customWidth="1"/>
-    <col min="3" max="4" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1397,7 +1428,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -1418,7 +1449,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -1440,15 +1471,15 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
-    <col min="2" max="2" width="6.21875" customWidth="1"/>
-    <col min="3" max="4" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1468,7 +1499,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -1489,7 +1520,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -1508,7 +1539,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -1527,7 +1558,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -1546,7 +1577,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -1565,7 +1596,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -1587,15 +1618,15 @@
       <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
-    <col min="2" max="2" width="6.21875" customWidth="1"/>
-    <col min="3" max="4" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="21.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="21.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1615,7 +1646,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -1636,7 +1667,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -1645,7 +1676,7 @@
         <v>8191</v>
       </c>
     </row>
-    <row r="34" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M34" t="s">
         <v>59</v>
       </c>
@@ -1663,18 +1694,18 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
-    <col min="2" max="2" width="6.21875" customWidth="1"/>
-    <col min="3" max="4" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="20.44140625" customWidth="1"/>
-    <col min="7" max="7" width="15.88671875" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="20.453125" customWidth="1"/>
+    <col min="7" max="7" width="15.90625" customWidth="1"/>
     <col min="8" max="8" width="28" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -1703,7 +1734,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -1733,7 +1764,7 @@
         <v>A84F</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>63</v>
       </c>
@@ -1764,7 +1795,7 @@
         <v>BEAF</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -1795,7 +1826,7 @@
         <v>BFFF</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="E10">
         <f>SUM(E2:E8)</f>
         <v>8192</v>
@@ -1814,15 +1845,15 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.21875" customWidth="1"/>
-    <col min="3" max="4" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="31.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1842,7 +1873,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -1863,7 +1894,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -1885,7 +1916,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>50</v>
       </c>
@@ -1907,7 +1938,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -1925,20 +1956,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84FE8641-C02D-4ECA-9797-EDC79FC57C57}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
-    <col min="2" max="2" width="6.21875" customWidth="1"/>
-    <col min="3" max="4" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.88671875" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1967,7 +1998,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -1997,7 +2028,7 @@
         <v>BEAF</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>62</v>
       </c>
@@ -2028,7 +2059,7 @@
         <v>BFFF</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="E9">
         <f>SUM(E2:E7)</f>
         <v>8192</v>
@@ -2048,14 +2079,14 @@
       <selection activeCell="A7" sqref="A7:E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
-    <col min="2" max="2" width="6.21875" customWidth="1"/>
-    <col min="3" max="4" width="11.44140625" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -2073,7 +2104,7 @@
       </c>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -2091,7 +2122,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -2110,7 +2141,7 @@
         <v>1275</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -2129,7 +2160,7 @@
         <v>1275</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -2148,7 +2179,7 @@
         <v>1275</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -2167,7 +2198,7 @@
         <v>1275</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -2186,7 +2217,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -2209,14 +2240,14 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
-    <col min="2" max="2" width="6.21875" customWidth="1"/>
-    <col min="3" max="4" width="11.44140625" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -2234,7 +2265,7 @@
       </c>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -2252,7 +2283,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -2272,7 +2303,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -2291,7 +2322,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -2310,12 +2341,12 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -2338,14 +2369,14 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
-    <col min="2" max="2" width="6.21875" customWidth="1"/>
-    <col min="3" max="4" width="11.44140625" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -2363,7 +2394,7 @@
       </c>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -2381,7 +2412,7 @@
         <v>1536</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -2400,7 +2431,7 @@
         <v>2040</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -2419,12 +2450,12 @@
         <v>2295</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -2447,13 +2478,13 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="60.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.5546875" customWidth="1"/>
+    <col min="1" max="1" width="60.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -2473,7 +2504,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -2495,7 +2526,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -2518,7 +2549,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -2541,7 +2572,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -2564,12 +2595,12 @@
         <v>7F4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -2578,7 +2609,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -2589,6 +2620,227 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C9D07F7-AEFD-4D2F-97E3-087A93BF23D8}">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="15.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>38400</v>
+      </c>
+      <c r="D2" t="str">
+        <f>DEC2HEX(HEX2DEC("00000"))</f>
+        <v>0</v>
+      </c>
+      <c r="E2" t="str">
+        <f t="shared" ref="E2:E6" si="0">DEC2HEX(HEX2DEC(D2)+C2-1)</f>
+        <v>95FF</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3">
+        <f>C2</f>
+        <v>38400</v>
+      </c>
+      <c r="C3">
+        <v>13360</v>
+      </c>
+      <c r="D3" t="str">
+        <f>DEC2HEX(B2 + C2)</f>
+        <v>9600</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" si="0"/>
+        <v>CA2F</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4">
+        <f>B3+C3</f>
+        <v>51760</v>
+      </c>
+      <c r="C4">
+        <v>1488</v>
+      </c>
+      <c r="D4" t="str">
+        <f>DEC2HEX(B3 + C3)</f>
+        <v>CA30</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>CFFF</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5">
+        <f>B4+C4</f>
+        <v>53248</v>
+      </c>
+      <c r="C5">
+        <v>2560</v>
+      </c>
+      <c r="D5" t="str">
+        <f>DEC2HEX(B4 + C4)</f>
+        <v>D000</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v>D9FF</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6">
+        <f>B5+C5</f>
+        <v>55808</v>
+      </c>
+      <c r="C6">
+        <v>2561</v>
+      </c>
+      <c r="D6" t="str">
+        <f>DEC2HEX(B5 + C5)</f>
+        <v>DA00</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="0"/>
+        <v>E400</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7">
+        <f>B6+C6</f>
+        <v>58369</v>
+      </c>
+      <c r="C7">
+        <v>1023</v>
+      </c>
+      <c r="D7" t="str">
+        <f>DEC2HEX(B6 + C6)</f>
+        <v>E401</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" ref="E7" si="1">DEC2HEX(HEX2DEC(D7)+C7-1)</f>
+        <v>E7FF</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8">
+        <f>B7+C7</f>
+        <v>59392</v>
+      </c>
+      <c r="C8">
+        <v>60079</v>
+      </c>
+      <c r="D8" t="str">
+        <f>DEC2HEX(B7 + C7)</f>
+        <v>E800</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" ref="E8" si="2">DEC2HEX(HEX2DEC(D8)+C8-1)</f>
+        <v>1D2AE</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9">
+        <f>B8+C8</f>
+        <v>119471</v>
+      </c>
+      <c r="C9">
+        <v>10000</v>
+      </c>
+      <c r="D9" t="str">
+        <f>DEC2HEX(B8 + C8)</f>
+        <v>1D2AF</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" ref="E9" si="3">DEC2HEX(HEX2DEC(D9)+C9-1)</f>
+        <v>1F9BE</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12">
+        <f>SUM(C2:C9)</f>
+        <v>129471</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13">
+        <v>129471</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14">
+        <f>C13-C12</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -2598,7 +2850,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2612,16 +2864,16 @@
       <selection activeCell="A2" sqref="A2:F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="56.77734375" customWidth="1"/>
-    <col min="2" max="2" width="6.21875" customWidth="1"/>
-    <col min="3" max="4" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.88671875" customWidth="1"/>
+    <col min="1" max="1" width="56.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -2647,7 +2899,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>64</v>
       </c>
@@ -2676,7 +2928,7 @@
         <v>BD2D</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>66</v>
       </c>
@@ -2703,7 +2955,7 @@
         <v>BDD4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>67</v>
       </c>
@@ -2729,19 +2981,19 @@
         <v>BF22</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E5">
         <f>SUM(E2+E4)</f>
         <v>7804</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:8" ht="253.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:8" ht="253" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
@@ -2764,15 +3016,15 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
-    <col min="2" max="2" width="6.21875" customWidth="1"/>
-    <col min="3" max="4" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="21.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="21.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -2792,7 +3044,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -2813,7 +3065,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -2836,15 +3088,15 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
-    <col min="2" max="2" width="6.21875" customWidth="1"/>
-    <col min="3" max="4" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="21.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="21.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -2864,7 +3116,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -2885,7 +3137,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -2907,15 +3159,15 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
-    <col min="2" max="2" width="6.21875" customWidth="1"/>
-    <col min="3" max="4" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="21.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="21.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -2935,7 +3187,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -2956,7 +3208,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -2964,7 +3216,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -2972,7 +3224,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -2980,7 +3232,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -3002,15 +3254,15 @@
       <selection activeCell="B3" sqref="B3:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
-    <col min="2" max="2" width="6.21875" customWidth="1"/>
-    <col min="3" max="4" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="21.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="21.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -3030,7 +3282,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -3051,7 +3303,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -3073,15 +3325,15 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
-    <col min="2" max="2" width="6.21875" customWidth="1"/>
-    <col min="3" max="4" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="21.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="21.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -3101,7 +3353,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -3122,7 +3374,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Created method for generating tiles for layer 1, untested
</commit_message>
<xml_diff>
--- a/docs/allocation.xlsx
+++ b/docs/allocation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{114C7692-8438-45FE-9B4E-7596E6C3E396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A90EA51-7FF4-423F-8C66-36AF3511AF09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" firstSheet="14" activeTab="25" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="83">
   <si>
     <t>Type</t>
   </si>
@@ -315,9 +315,6 @@
   </si>
   <si>
     <t>Sprites</t>
-  </si>
-  <si>
-    <t>Volatile Buffer</t>
   </si>
 </sst>
 </file>
@@ -2625,10 +2622,10 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C9D07F7-AEFD-4D2F-97E3-087A93BF23D8}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2685,7 +2682,7 @@
         <v>13360</v>
       </c>
       <c r="D3" t="str">
-        <f>DEC2HEX(B2 + C2)</f>
+        <f t="shared" ref="D3:D6" si="1">DEC2HEX(B2 + C2)</f>
         <v>9600</v>
       </c>
       <c r="E3" t="str">
@@ -2698,14 +2695,14 @@
         <v>58</v>
       </c>
       <c r="B4">
-        <f>B3+C3</f>
+        <f t="shared" ref="B4:B6" si="2">B3+C3</f>
         <v>51760</v>
       </c>
       <c r="C4">
         <v>1488</v>
       </c>
       <c r="D4" t="str">
-        <f>DEC2HEX(B3 + C3)</f>
+        <f t="shared" si="1"/>
         <v>CA30</v>
       </c>
       <c r="E4" t="str">
@@ -2718,14 +2715,14 @@
         <v>77</v>
       </c>
       <c r="B5">
-        <f>B4+C4</f>
+        <f t="shared" si="2"/>
         <v>53248</v>
       </c>
       <c r="C5">
         <v>2560</v>
       </c>
       <c r="D5" t="str">
-        <f>DEC2HEX(B4 + C4)</f>
+        <f t="shared" si="1"/>
         <v>D000</v>
       </c>
       <c r="E5" t="str">
@@ -2738,105 +2735,65 @@
         <v>78</v>
       </c>
       <c r="B6">
-        <f>B5+C5</f>
+        <f t="shared" si="2"/>
         <v>55808</v>
       </c>
       <c r="C6">
-        <v>2561</v>
+        <v>4096</v>
       </c>
       <c r="D6" t="str">
-        <f>DEC2HEX(B5 + C5)</f>
+        <f t="shared" si="1"/>
         <v>DA00</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
-        <v>E400</v>
+        <v>E9FF</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="B7">
-        <f>B6+C6</f>
-        <v>58369</v>
+        <f t="shared" ref="B7" si="3">B6+C6</f>
+        <v>59904</v>
       </c>
       <c r="C7">
-        <v>1023</v>
+        <v>4097</v>
       </c>
       <c r="D7" t="str">
-        <f>DEC2HEX(B6 + C6)</f>
-        <v>E401</v>
+        <f t="shared" ref="D7" si="4">DEC2HEX(B6 + C6)</f>
+        <v>EA00</v>
       </c>
       <c r="E7" t="str">
-        <f t="shared" ref="E7" si="1">DEC2HEX(HEX2DEC(D7)+C7-1)</f>
-        <v>E7FF</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>82</v>
-      </c>
-      <c r="B8">
-        <f>B7+C7</f>
-        <v>59392</v>
-      </c>
-      <c r="C8">
-        <v>60079</v>
-      </c>
-      <c r="D8" t="str">
-        <f>DEC2HEX(B7 + C7)</f>
-        <v>E800</v>
-      </c>
-      <c r="E8" t="str">
-        <f t="shared" ref="E8" si="2">DEC2HEX(HEX2DEC(D8)+C8-1)</f>
-        <v>1D2AE</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>83</v>
-      </c>
-      <c r="B9">
-        <f>B8+C8</f>
-        <v>119471</v>
-      </c>
-      <c r="C9">
-        <v>10000</v>
-      </c>
-      <c r="D9" t="str">
-        <f>DEC2HEX(B8 + C8)</f>
-        <v>1D2AF</v>
-      </c>
-      <c r="E9" t="str">
-        <f t="shared" ref="E9" si="3">DEC2HEX(HEX2DEC(D9)+C9-1)</f>
-        <v>1F9BE</v>
+        <f t="shared" ref="E7" si="5">DEC2HEX(HEX2DEC(D7)+C7-1)</f>
+        <v>FA00</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10">
+        <f>SUM(C2:C7)</f>
+        <v>64001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11">
+        <v>129471</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C12">
-        <f>SUM(C2:C9)</f>
-        <v>129471</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B13" t="s">
-        <v>80</v>
-      </c>
-      <c r="C13">
-        <v>129471</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C14">
-        <f>C13-C12</f>
-        <v>0</v>
+        <f>C11-C10</f>
+        <v>65470</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created tile layer of letters for text.
</commit_message>
<xml_diff>
--- a/docs/allocation.xlsx
+++ b/docs/allocation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A90EA51-7FF4-423F-8C66-36AF3511AF09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF986389-A6FB-423A-AAAA-E390BF038B3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" firstSheet="14" activeTab="25" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
+    <workbookView minimized="1" xWindow="3740" yWindow="3730" windowWidth="15820" windowHeight="6820" firstSheet="14" activeTab="25" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic (Bank 0x13 - 0x26)" sheetId="2" r:id="rId1"/>
@@ -2625,13 +2625,14 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="15.81640625" customWidth="1"/>
+    <col min="6" max="6" width="9.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -2798,6 +2799,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Created top and right border chars
</commit_message>
<xml_diff>
--- a/docs/allocation.xlsx
+++ b/docs/allocation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF986389-A6FB-423A-AAAA-E390BF038B3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0817270A-5260-4FBB-A1CF-1BAC1D9DAE56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3740" yWindow="3730" windowWidth="15820" windowHeight="6820" firstSheet="14" activeTab="25" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" activeTab="6" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic (Bank 0x13 - 0x26)" sheetId="2" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="84">
   <si>
     <t>Type</t>
   </si>
@@ -315,6 +315,9 @@
   </si>
   <si>
     <t>Sprites</t>
+  </si>
+  <si>
+    <t>Interpolation Buffer</t>
   </si>
 </sst>
 </file>
@@ -1688,7 +1691,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection sqref="A1:I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2624,7 +2627,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C9D07F7-AEFD-4D2F-97E3-087A93BF23D8}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -3112,10 +3115,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{382A0DF3-A6E2-4E63-819F-0B238C4B218B}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3124,80 +3127,161 @@
     <col min="2" max="2" width="6.1796875" customWidth="1"/>
     <col min="3" max="4" width="11.453125" customWidth="1"/>
     <col min="6" max="6" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>30</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2">
+        <v>5191</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f>C2*D2</f>
+        <v>5191</v>
+      </c>
+      <c r="G2">
+        <f>B2+C2-1</f>
+        <v>5190</v>
+      </c>
+      <c r="H2" t="str">
+        <f>DEC2HEX(B2+40960)</f>
+        <v>A000</v>
+      </c>
+      <c r="I2" t="str">
+        <f>DEC2HEX(G2+40960)</f>
+        <v>B446</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3">
+        <f>G2+1</f>
+        <v>5191</v>
+      </c>
+      <c r="C3">
+        <v>1001</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <f>C3*D3</f>
+        <v>1001</v>
+      </c>
+      <c r="G3">
+        <f>B3+C3-1</f>
+        <v>6191</v>
+      </c>
+      <c r="H3" t="str">
+        <f>DEC2HEX(B3+40960)</f>
+        <v>B447</v>
+      </c>
+      <c r="I3" t="str">
+        <f>DEC2HEX(G3+40960)</f>
+        <v>B82F</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4">
+        <f>G3+1</f>
+        <v>6192</v>
+      </c>
+      <c r="C4">
+        <v>2000</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <f>C4*D4</f>
+        <v>2000</v>
+      </c>
+      <c r="G4">
+        <f>B4+C4-1</f>
+        <v>8191</v>
+      </c>
+      <c r="H4" t="str">
+        <f>DEC2HEX(B4+40960)</f>
+        <v>B830</v>
+      </c>
+      <c r="I4" t="str">
+        <f>DEC2HEX(G4+40960)</f>
+        <v>BFFF</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
         <v>36</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="str">
-        <f>C2</f>
-        <v>TBD</v>
-      </c>
-      <c r="F2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E12">
         <f>SUM(E2:E10)</f>
-        <v>0</v>
+        <v>8192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Now waiting for next Irq counter instead of state
</commit_message>
<xml_diff>
--- a/docs/allocation.xlsx
+++ b/docs/allocation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0817270A-5260-4FBB-A1CF-1BAC1D9DAE56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD5B8988-A647-44EC-BFF3-9F9A0943C417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" activeTab="6" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="85">
   <si>
     <t>Type</t>
   </si>
@@ -318,6 +318,9 @@
   </si>
   <si>
     <t>Interpolation Buffer</t>
+  </si>
+  <si>
+    <t>Message Buffer</t>
   </si>
 </sst>
 </file>
@@ -3118,7 +3121,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3191,7 +3194,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="B3">
         <f>G2+1</f>

</xml_diff>

<commit_message>
text buffer is now tracked by the compiler
</commit_message>
<xml_diff>
--- a/docs/allocation.xlsx
+++ b/docs/allocation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD5B8988-A647-44EC-BFF3-9F9A0943C417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3AD936E-58FF-488E-AE79-5594469CD03D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" activeTab="6" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="85">
   <si>
     <t>Type</t>
   </si>
@@ -317,10 +317,10 @@
     <t>Sprites</t>
   </si>
   <si>
-    <t>Interpolation Buffer</t>
-  </si>
-  <si>
-    <t>Message Buffer</t>
+    <t>This bank is for text processing and includes the text processing buffers. The address of the buffers (textbuffer1,textbuffer2 and interpolation buffer) and tracked by the compiler</t>
+  </si>
+  <si>
+    <t>code/buffers</t>
   </si>
 </sst>
 </file>
@@ -364,11 +364,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3118,10 +3121,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{382A0DF3-A6E2-4E63-819F-0B238C4B218B}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3164,24 +3167,24 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>84</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>5191</v>
+        <v>8192</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2">
         <f>C2*D2</f>
-        <v>5191</v>
+        <v>8192</v>
       </c>
       <c r="G2">
         <f>B2+C2-1</f>
-        <v>5190</v>
+        <v>8191</v>
       </c>
       <c r="H2" t="str">
         <f>DEC2HEX(B2+40960)</f>
@@ -3189,102 +3192,45 @@
       </c>
       <c r="I2" t="str">
         <f>DEC2HEX(G2+40960)</f>
-        <v>B446</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B3">
-        <f>G2+1</f>
-        <v>5191</v>
-      </c>
-      <c r="C3">
-        <v>1001</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <f>C3*D3</f>
-        <v>1001</v>
-      </c>
-      <c r="G3">
-        <f>B3+C3-1</f>
-        <v>6191</v>
-      </c>
-      <c r="H3" t="str">
-        <f>DEC2HEX(B3+40960)</f>
-        <v>B447</v>
-      </c>
-      <c r="I3" t="str">
-        <f>DEC2HEX(G3+40960)</f>
-        <v>B82F</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B4">
-        <f>G3+1</f>
-        <v>6192</v>
-      </c>
-      <c r="C4">
-        <v>2000</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <f>C4*D4</f>
-        <v>2000</v>
-      </c>
-      <c r="G4">
-        <f>B4+C4-1</f>
-        <v>8191</v>
-      </c>
-      <c r="H4" t="str">
-        <f>DEC2HEX(B4+40960)</f>
-        <v>B830</v>
-      </c>
-      <c r="I4" t="str">
-        <f>DEC2HEX(G4+40960)</f>
         <v>BFFF</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" t="s">
-        <v>36</v>
-      </c>
-    </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
+      <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E12">
-        <f>SUM(E2:E10)</f>
+      <c r="E10">
+        <f>SUM(E2:E8)</f>
         <v>8192</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="145" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Now loading cel metadata
</commit_message>
<xml_diff>
--- a/docs/allocation.xlsx
+++ b/docs/allocation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3AD936E-58FF-488E-AE79-5594469CD03D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D04DCE-8E1C-4B55-8667-1DA83DD1D4BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" activeTab="6" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" firstSheet="12" activeTab="22" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic (Bank 0x13 - 0x26)" sheetId="2" r:id="rId1"/>
@@ -364,14 +364,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2242,8 +2239,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A86A6CAE-A2FB-4700-AF3B-F451BF94FBFE}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2337,14 +2334,14 @@
         <v>4623</v>
       </c>
       <c r="C5">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D5">
         <v>256</v>
       </c>
       <c r="E5">
         <f t="shared" ref="E5" si="3">C5*D5</f>
-        <v>2048</v>
+        <v>2560</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -2358,7 +2355,7 @@
       </c>
       <c r="E13">
         <f>SUM(E2:E11)</f>
-        <v>6668</v>
+        <v>7180</v>
       </c>
     </row>
   </sheetData>
@@ -3123,7 +3120,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{382A0DF3-A6E2-4E63-819F-0B238C4B218B}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -3229,7 +3226,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="145" x14ac:dyDescent="0.35">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>83</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added structs for multi sprite slots
</commit_message>
<xml_diff>
--- a/docs/allocation.xlsx
+++ b/docs/allocation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19AC51E8-E6D9-4024-BA68-49BD7236F0FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE7436F4-4694-43FE-8E5D-71FD1FD9C160}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" firstSheet="12" activeTab="25" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="90">
   <si>
     <t>Type</t>
   </si>
@@ -321,6 +321,21 @@
   </si>
   <si>
     <t>code/buffers</t>
+  </si>
+  <si>
+    <t>No Sprites</t>
+  </si>
+  <si>
+    <t>Sprite Width</t>
+  </si>
+  <si>
+    <t>Average Loop Length</t>
+  </si>
+  <si>
+    <t>Average Loop limit</t>
+  </si>
+  <si>
+    <t>Sprites Secondary</t>
   </si>
 </sst>
 </file>
@@ -364,13 +379,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2628,10 +2644,10 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C9D07F7-AEFD-4D2F-97E3-087A93BF23D8}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2640,9 +2656,12 @@
     <col min="3" max="3" width="10.90625" customWidth="1"/>
     <col min="4" max="5" width="15.81640625" customWidth="1"/>
     <col min="6" max="6" width="9.90625" customWidth="1"/>
+    <col min="7" max="7" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -2658,8 +2677,20 @@
       <c r="E1" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>75</v>
       </c>
@@ -2677,8 +2708,22 @@
         <f t="shared" ref="E2:E6" si="0">DEC2HEX(HEX2DEC(D2)+C2-1)</f>
         <v>95FF</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F2">
+        <f>C7/((G2*G2)/2)</f>
+        <v>2173.96875</v>
+      </c>
+      <c r="G2" s="4">
+        <v>8</v>
+      </c>
+      <c r="H2">
+        <v>7</v>
+      </c>
+      <c r="I2">
+        <f>F2/H2</f>
+        <v>310.56696428571428</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>76</v>
       </c>
@@ -2697,13 +2742,27 @@
         <f t="shared" si="0"/>
         <v>CA2F</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F3">
+        <f>C7/((G3*G3)/2)</f>
+        <v>543.4921875</v>
+      </c>
+      <c r="G3">
+        <v>16</v>
+      </c>
+      <c r="H3">
+        <v>7</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I5" si="2">F3/H3</f>
+        <v>77.641741071428569</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B6" si="2">B3+C3</f>
+        <f t="shared" ref="B4:B6" si="3">B3+C3</f>
         <v>51760</v>
       </c>
       <c r="C4">
@@ -2717,13 +2776,27 @@
         <f t="shared" si="0"/>
         <v>CFFF</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F4">
+        <f>C7/((G4*G4)/2)</f>
+        <v>135.873046875</v>
+      </c>
+      <c r="G4">
+        <v>32</v>
+      </c>
+      <c r="H4">
+        <v>7</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="2"/>
+        <v>19.410435267857142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>77</v>
       </c>
       <c r="B5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>53248</v>
       </c>
       <c r="C5">
@@ -2737,13 +2810,27 @@
         <f t="shared" si="0"/>
         <v>D9FF</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F5">
+        <f>C7/((G5*G5)/2)</f>
+        <v>33.96826171875</v>
+      </c>
+      <c r="G5">
+        <v>64</v>
+      </c>
+      <c r="H5">
+        <v>7</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="2"/>
+        <v>4.8526088169642856</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>78</v>
       </c>
       <c r="B6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>55808</v>
       </c>
       <c r="C6">
@@ -2758,27 +2845,27 @@
         <v>E9FF</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>82</v>
       </c>
       <c r="B7">
-        <f t="shared" ref="B7" si="3">B6+C6</f>
+        <f t="shared" ref="B7" si="4">B6+C6</f>
         <v>59904</v>
       </c>
       <c r="C7">
         <v>69567</v>
       </c>
       <c r="D7" t="str">
-        <f t="shared" ref="D7" si="4">DEC2HEX(B6 + C6)</f>
+        <f t="shared" ref="D7" si="5">DEC2HEX(B6 + C6)</f>
         <v>EA00</v>
       </c>
       <c r="E7" t="str">
-        <f t="shared" ref="E7" si="5">DEC2HEX(HEX2DEC(D7)+C7-1)</f>
+        <f t="shared" ref="E7" si="6">DEC2HEX(HEX2DEC(D7)+C7-1)</f>
         <v>1F9BE</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>79</v>
       </c>
@@ -2787,7 +2874,7 @@
         <v>129471</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>80</v>
       </c>
@@ -2795,7 +2882,7 @@
         <v>129471</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>81</v>
       </c>

</xml_diff>

<commit_message>
Moved lru cache off bank e onto bank 4 freeing up space for sprite stuff
</commit_message>
<xml_diff>
--- a/docs/allocation.xlsx
+++ b/docs/allocation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F64DD94-BE4E-4A6B-BD07-C6A7B1FFF9F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE18B25-D979-42FE-AC24-8594F4E95E9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" firstSheet="12" activeTab="25" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
+    <workbookView minimized="1" xWindow="12060" yWindow="3250" windowWidth="7160" windowHeight="6960" firstSheet="12" activeTab="17" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic (Bank 0x13 - 0x26)" sheetId="2" r:id="rId1"/>
@@ -30,15 +30,14 @@
     <sheet name="Bank0xB" sheetId="15" r:id="rId15"/>
     <sheet name="Bank0xC" sheetId="16" r:id="rId16"/>
     <sheet name="Bank0xD" sheetId="17" r:id="rId17"/>
-    <sheet name="Bank0xE" sheetId="18" r:id="rId18"/>
-    <sheet name="Bank0xF" sheetId="21" r:id="rId19"/>
-    <sheet name="Bank0x10" sheetId="19" r:id="rId20"/>
-    <sheet name="Bank0x11" sheetId="24" r:id="rId21"/>
-    <sheet name="BANK0x3C" sheetId="1" r:id="rId22"/>
-    <sheet name="BANK0x3D" sheetId="5" r:id="rId23"/>
-    <sheet name="BANK0x3E" sheetId="20" r:id="rId24"/>
-    <sheet name="Golden" sheetId="4" r:id="rId25"/>
-    <sheet name="Vera" sheetId="27" r:id="rId26"/>
+    <sheet name="Bank0xF" sheetId="21" r:id="rId18"/>
+    <sheet name="Bank0x10" sheetId="19" r:id="rId19"/>
+    <sheet name="Bank0x11" sheetId="24" r:id="rId20"/>
+    <sheet name="BANK0x3C" sheetId="1" r:id="rId21"/>
+    <sheet name="BANK0x3D" sheetId="5" r:id="rId22"/>
+    <sheet name="BANK0x3E" sheetId="20" r:id="rId23"/>
+    <sheet name="Golden" sheetId="4" r:id="rId24"/>
+    <sheet name="Vera" sheetId="27" r:id="rId25"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -58,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="86">
   <si>
     <t>Type</t>
   </si>
@@ -178,21 +177,6 @@
   </si>
   <si>
     <t>View Code</t>
-  </si>
-  <si>
-    <t>Cache Code</t>
-  </si>
-  <si>
-    <t>lruCache Logic</t>
-  </si>
-  <si>
-    <t>lruCache View</t>
-  </si>
-  <si>
-    <t>lruCache Logic Data</t>
-  </si>
-  <si>
-    <t>IruCache View Data</t>
   </si>
   <si>
     <t>parameters</t>
@@ -761,7 +745,7 @@
         <v>8000</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -788,7 +772,7 @@
         <v>8000</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F3">
         <f>D3/8000</f>
@@ -818,7 +802,7 @@
         <v>48000</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F4">
         <v>6</v>
@@ -847,7 +831,7 @@
         <v>48000</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F5">
         <v>6</v>
@@ -876,7 +860,7 @@
         <v>48000</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F6">
         <f>D6/8000</f>
@@ -971,7 +955,7 @@
         <v>8191</v>
       </c>
       <c r="F2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1042,7 +1026,7 @@
         <v>8191</v>
       </c>
       <c r="F2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1113,7 +1097,7 @@
         <v>8191</v>
       </c>
       <c r="F2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1485,157 +1469,10 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1B96CF0-432F-4A3E-940D-86E08F6940C7}">
-  <dimension ref="A1:F12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="19.81640625" customWidth="1"/>
-    <col min="2" max="2" width="6.1796875" customWidth="1"/>
-    <col min="3" max="4" width="11.453125" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>682</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <f>C2</f>
-        <v>682</v>
-      </c>
-      <c r="F2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3">
-        <f>8191 -E3</f>
-        <v>8183</v>
-      </c>
-      <c r="C3">
-        <v>8</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <f>C3 * D3</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4">
-        <f>B3-E4</f>
-        <v>8173</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>10</v>
-      </c>
-      <c r="E4">
-        <f>C4 * D4</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5">
-        <f>B4-E5</f>
-        <v>8165</v>
-      </c>
-      <c r="C5">
-        <v>8</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <f>C5 * D5</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6">
-        <f>B5-E6</f>
-        <v>8145</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>20</v>
-      </c>
-      <c r="E6">
-        <f>C6 * D6</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12">
-        <f>SUM(E2:E10)</f>
-        <v>728</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{470FF23A-2CF2-4342-A127-6A0CAC1D7ECC}">
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
@@ -1699,7 +1536,122 @@
     </row>
     <row r="34" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M34" t="s">
-        <v>59</v>
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C39777F-CEF0-4425-930E-295AE7C473DC}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="31.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="31.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1586</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f>C2</f>
+        <v>1586</v>
+      </c>
+      <c r="F2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3">
+        <f>B4-E3</f>
+        <v>7971</v>
+      </c>
+      <c r="C3">
+        <v>186</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <f>C3*D3</f>
+        <v>186</v>
+      </c>
+      <c r="F3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4">
+        <f>8192-E4</f>
+        <v>8157</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <f>C4*D4</f>
+        <v>35</v>
+      </c>
+      <c r="F4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <f>SUM(E2:E10)</f>
+        <v>1807</v>
       </c>
     </row>
   </sheetData>
@@ -1746,13 +1698,13 @@
         <v>37</v>
       </c>
       <c r="G1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="I1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -1787,7 +1739,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B3">
         <f>G2+1</f>
@@ -1818,7 +1770,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B4">
         <f>G3+1</f>
@@ -1859,121 +1811,6 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C39777F-CEF0-4425-930E-295AE7C473DC}">
-  <dimension ref="A1:F12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="31.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.1796875" customWidth="1"/>
-    <col min="3" max="4" width="11.453125" customWidth="1"/>
-    <col min="6" max="6" width="31.36328125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>1586</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <f>C2</f>
-        <v>1586</v>
-      </c>
-      <c r="F2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3">
-        <f>B4-E3</f>
-        <v>7971</v>
-      </c>
-      <c r="C3">
-        <v>186</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <f>C3*D3</f>
-        <v>186</v>
-      </c>
-      <c r="F3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4">
-        <f>8192-E4</f>
-        <v>8157</v>
-      </c>
-      <c r="C4">
-        <v>7</v>
-      </c>
-      <c r="D4">
-        <v>5</v>
-      </c>
-      <c r="E4">
-        <f>C4*D4</f>
-        <v>35</v>
-      </c>
-      <c r="F4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12">
-        <f>SUM(E2:E10)</f>
-        <v>1807</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84FE8641-C02D-4ECA-9797-EDC79FC57C57}">
   <dimension ref="A1:I9"/>
   <sheetViews>
@@ -2010,13 +1847,13 @@
         <v>37</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -2051,7 +1888,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B3">
         <f>G2+1</f>
@@ -2092,7 +1929,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8A806B9-8F96-4CFC-8F80-C6046C4BB66C}">
   <dimension ref="A1:F13"/>
   <sheetViews>
@@ -2253,7 +2090,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A86A6CAE-A2FB-4700-AF3B-F451BF94FBFE}">
   <dimension ref="A1:F13"/>
   <sheetViews>
@@ -2364,7 +2201,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -2382,7 +2219,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1ECB7A9-D68D-4611-9022-3CBE081861CE}">
   <dimension ref="A1:F13"/>
   <sheetViews>
@@ -2417,7 +2254,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -2473,7 +2310,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -2491,7 +2328,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF57E188-51E7-49EE-9F4F-07D9A5354CD1}">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -2522,7 +2359,7 @@
         <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -2595,7 +2432,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B5">
         <f>B4+ E4+1</f>
@@ -2618,7 +2455,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -2644,11 +2481,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C9D07F7-AEFD-4D2F-97E3-087A93BF23D8}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -2675,27 +2512,27 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -2728,7 +2565,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B3">
         <f>C2</f>
@@ -2762,7 +2599,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B4">
         <f t="shared" ref="B4:B6" si="3">B3+C3</f>
@@ -2796,7 +2633,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B5">
         <f t="shared" si="3"/>
@@ -2830,7 +2667,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B6">
         <f t="shared" si="3"/>
@@ -2850,7 +2687,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B7">
         <f t="shared" ref="B7" si="4">B6+C6</f>
@@ -2870,7 +2707,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C9">
         <f>C7+C4</f>
@@ -2879,7 +2716,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C10">
         <f>SUM(C2:C7)</f>
@@ -2888,7 +2725,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C11">
         <v>129471</v>
@@ -2896,7 +2733,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C12">
         <f>C11-C10</f>
@@ -2958,15 +2795,15 @@
         <v>37</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -2982,7 +2819,7 @@
         <v>7470</v>
       </c>
       <c r="F2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G2" t="str">
         <f>DEC2HEX(HEX2DEC("A000"))</f>
@@ -2995,7 +2832,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B3">
         <f>C2</f>
@@ -3022,7 +2859,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B4">
         <f>B3+E3</f>
@@ -3055,7 +2892,7 @@
     <row r="6" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="7" spans="1:8" ht="253" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
@@ -3253,18 +3090,18 @@
         <v>37</v>
       </c>
       <c r="G1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="I1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -3327,7 +3164,7 @@
     </row>
     <row r="13" spans="1:9" ht="145" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First cut of metadata initialization
</commit_message>
<xml_diff>
--- a/docs/allocation.xlsx
+++ b/docs/allocation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE18B25-D979-42FE-AC24-8594F4E95E9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97BAA77B-3D97-4BE0-9C05-4A4AE57C86E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="12060" yWindow="3250" windowWidth="7160" windowHeight="6960" firstSheet="12" activeTab="17" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" firstSheet="11" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic (Bank 0x13 - 0x26)" sheetId="2" r:id="rId1"/>
@@ -689,8 +689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{355DE0EA-5B2C-4635-84EE-7D1B81ED29C7}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1472,7 +1472,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{470FF23A-2CF2-4342-A127-6A0CAC1D7ECC}">
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
@@ -1934,7 +1934,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:E8"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2095,7 +2095,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2189,14 +2189,14 @@
         <v>4623</v>
       </c>
       <c r="C5">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D5">
         <v>256</v>
       </c>
       <c r="E5">
         <f t="shared" ref="E5" si="3">C5*D5</f>
-        <v>2560</v>
+        <v>3328</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -2210,7 +2210,7 @@
       </c>
       <c r="E13">
         <f>SUM(E2:E11)</f>
-        <v>7180</v>
+        <v>7948</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Create vera slot calcuations and put them on objects
</commit_message>
<xml_diff>
--- a/docs/allocation.xlsx
+++ b/docs/allocation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97BAA77B-3D97-4BE0-9C05-4A4AE57C86E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF3BB3F-6D78-4576-8699-C257B95BA053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" firstSheet="11" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" firstSheet="11" activeTab="21" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic (Bank 0x13 - 0x26)" sheetId="2" r:id="rId1"/>
@@ -689,7 +689,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{355DE0EA-5B2C-4635-84EE-7D1B81ED29C7}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -2094,8 +2094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A86A6CAE-A2FB-4700-AF3B-F451BF94FBFE}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2189,14 +2189,14 @@
         <v>4623</v>
       </c>
       <c r="C5">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5">
         <v>256</v>
       </c>
       <c r="E5">
         <f t="shared" ref="E5" si="3">C5*D5</f>
-        <v>3328</v>
+        <v>3072</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -2210,7 +2210,7 @@
       </c>
       <c r="E13">
         <f>SUM(E2:E11)</f>
-        <v>7948</v>
+        <v>7692</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Now bulk allocating vera addresses for sprites
</commit_message>
<xml_diff>
--- a/docs/allocation.xlsx
+++ b/docs/allocation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF3BB3F-6D78-4576-8699-C257B95BA053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{460DBD9A-7D70-4234-9C94-F341C67EBC11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" firstSheet="11" activeTab="21" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
@@ -2095,7 +2095,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Fixed crash after ten minutes due to misssized memory allocation segment
</commit_message>
<xml_diff>
--- a/docs/allocation.xlsx
+++ b/docs/allocation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{460DBD9A-7D70-4234-9C94-F341C67EBC11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1DDCA2-9238-4EA6-98E4-769CBB681C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" firstSheet="11" activeTab="21" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="5490" windowWidth="7500" windowHeight="4730" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic (Bank 0x13 - 0x26)" sheetId="2" r:id="rId1"/>
@@ -689,8 +689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{355DE0EA-5B2C-4635-84EE-7D1B81ED29C7}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -824,11 +824,11 @@
         <v>3200</v>
       </c>
       <c r="C5">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D5">
         <f>B5*C5</f>
-        <v>48000</v>
+        <v>38400</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>55</v>
@@ -842,7 +842,7 @@
       </c>
       <c r="H5">
         <f>G5+C5 -1</f>
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -868,11 +868,11 @@
       </c>
       <c r="G6">
         <f>H5+1</f>
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="H6">
         <f>G6+C6 - 1</f>
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -885,11 +885,11 @@
       </c>
       <c r="C9">
         <f>SUM(C2:C6)</f>
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D9">
         <f>SUM(D2:D8)</f>
-        <v>160000</v>
+        <v>150400</v>
       </c>
       <c r="F9">
         <f>SUM(F2:F6)</f>
@@ -2094,7 +2094,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A86A6CAE-A2FB-4700-AF3B-F451BF94FBFE}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Now allocating a fixed amount when splitting, which is large enough for no overrun
</commit_message>
<xml_diff>
--- a/docs/allocation.xlsx
+++ b/docs/allocation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1DDCA2-9238-4EA6-98E4-769CBB681C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC068A5-9723-4E61-933F-AAC00EF84FEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="5490" windowWidth="7500" windowHeight="4730" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic (Bank 0x13 - 0x26)" sheetId="2" r:id="rId1"/>
@@ -690,7 +690,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -821,14 +821,14 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>3200</v>
+        <v>4000</v>
       </c>
       <c r="C5">
         <v>12</v>
       </c>
       <c r="D5">
         <f>B5*C5</f>
-        <v>38400</v>
+        <v>48000</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>55</v>
@@ -881,7 +881,7 @@
       </c>
       <c r="B9">
         <f>SUM(B2:B8)</f>
-        <v>13060</v>
+        <v>13860</v>
       </c>
       <c r="C9">
         <f>SUM(C2:C6)</f>
@@ -889,7 +889,7 @@
       </c>
       <c r="D9">
         <f>SUM(D2:D8)</f>
-        <v>150400</v>
+        <v>160000</v>
       </c>
       <c r="F9">
         <f>SUM(F2:F6)</f>

</xml_diff>

<commit_message>
Revert "Now allocating a fixed amount when splitting, which is large enough for no overrun"
This reverts commit ebd2c0d7df8ae32cd070a17aa19b29e4b9bd4b18.
</commit_message>
<xml_diff>
--- a/docs/allocation.xlsx
+++ b/docs/allocation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC068A5-9723-4E61-933F-AAC00EF84FEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1DDCA2-9238-4EA6-98E4-769CBB681C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="5490" windowWidth="7500" windowHeight="4730" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic (Bank 0x13 - 0x26)" sheetId="2" r:id="rId1"/>
@@ -690,7 +690,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -821,14 +821,14 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>4000</v>
+        <v>3200</v>
       </c>
       <c r="C5">
         <v>12</v>
       </c>
       <c r="D5">
         <f>B5*C5</f>
-        <v>48000</v>
+        <v>38400</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>55</v>
@@ -881,7 +881,7 @@
       </c>
       <c r="B9">
         <f>SUM(B2:B8)</f>
-        <v>13860</v>
+        <v>13060</v>
       </c>
       <c r="C9">
         <f>SUM(C2:C6)</f>
@@ -889,7 +889,7 @@
       </c>
       <c r="D9">
         <f>SUM(D2:D8)</f>
-        <v>160000</v>
+        <v>150400</v>
       </c>
       <c r="F9">
         <f>SUM(F2:F6)</f>

</xml_diff>

<commit_message>
Revert "Revert "Now allocating a fixed amount when splitting, which is large enough for no overrun""
This reverts commit ee4300b79709315a3437f0819d767459613dbcf1.
</commit_message>
<xml_diff>
--- a/docs/allocation.xlsx
+++ b/docs/allocation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1DDCA2-9238-4EA6-98E4-769CBB681C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC068A5-9723-4E61-933F-AAC00EF84FEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="5490" windowWidth="7500" windowHeight="4730" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic (Bank 0x13 - 0x26)" sheetId="2" r:id="rId1"/>
@@ -690,7 +690,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -821,14 +821,14 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>3200</v>
+        <v>4000</v>
       </c>
       <c r="C5">
         <v>12</v>
       </c>
       <c r="D5">
         <f>B5*C5</f>
-        <v>38400</v>
+        <v>48000</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>55</v>
@@ -881,7 +881,7 @@
       </c>
       <c r="B9">
         <f>SUM(B2:B8)</f>
-        <v>13060</v>
+        <v>13860</v>
       </c>
       <c r="C9">
         <f>SUM(C2:C6)</f>
@@ -889,7 +889,7 @@
       </c>
       <c r="D9">
         <f>SUM(D2:D8)</f>
-        <v>150400</v>
+        <v>160000</v>
       </c>
       <c r="F9">
         <f>SUM(F2:F6)</f>

</xml_diff>

<commit_message>
Moved loadedPictures to bss for easy allocation and to free up the bank
</commit_message>
<xml_diff>
--- a/docs/allocation.xlsx
+++ b/docs/allocation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC068A5-9723-4E61-933F-AAC00EF84FEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD63415F-EE79-45DE-9581-D2927FFC47D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" firstSheet="8" activeTab="21" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic (Bank 0x13 - 0x26)" sheetId="2" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="78">
   <si>
     <t>Type</t>
   </si>
@@ -104,21 +104,6 @@
     <t>Start</t>
   </si>
   <si>
-    <t>Allocation Array</t>
-  </si>
-  <si>
-    <t>logDir</t>
-  </si>
-  <si>
-    <t>picDir</t>
-  </si>
-  <si>
-    <t>soundDir</t>
-  </si>
-  <si>
-    <t>viewDir</t>
-  </si>
-  <si>
     <t>logicEntry</t>
   </si>
   <si>
@@ -143,12 +128,6 @@
     <t>workArea</t>
   </si>
   <si>
-    <t>menu</t>
-  </si>
-  <si>
-    <t>menuChild</t>
-  </si>
-  <si>
     <t>code</t>
   </si>
   <si>
@@ -159,12 +138,6 @@
   </si>
   <si>
     <t>getNumTemp</t>
-  </si>
-  <si>
-    <t>viewTab</t>
-  </si>
-  <si>
-    <t>loadedView</t>
   </si>
   <si>
     <t>TBD</t>
@@ -323,6 +296,9 @@
   </si>
   <si>
     <t>Sprites Small</t>
+  </si>
+  <si>
+    <t>vacant</t>
   </si>
 </sst>
 </file>
@@ -366,13 +342,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -689,7 +666,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{355DE0EA-5B2C-4635-84EE-7D1B81ED29C7}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
@@ -745,7 +722,7 @@
         <v>8000</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -772,7 +749,7 @@
         <v>8000</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="F3">
         <f>D3/8000</f>
@@ -802,7 +779,7 @@
         <v>48000</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F4">
         <v>6</v>
@@ -831,7 +808,7 @@
         <v>48000</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="F5">
         <v>6</v>
@@ -860,7 +837,7 @@
         <v>48000</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="F6">
         <f>D6/8000</f>
@@ -932,15 +909,15 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -955,7 +932,7 @@
         <v>8191</v>
       </c>
       <c r="F2" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1002,15 +979,15 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1026,7 +1003,7 @@
         <v>8191</v>
       </c>
       <c r="F2" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1073,15 +1050,15 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1097,7 +1074,7 @@
         <v>8191</v>
       </c>
       <c r="F2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1144,15 +1121,15 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1168,7 +1145,7 @@
         <v>3586</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1215,15 +1192,15 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1239,7 +1216,7 @@
         <v>5123</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1286,15 +1263,15 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1310,7 +1287,7 @@
         <v>3723</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1357,15 +1334,15 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1380,7 +1357,7 @@
         <v>3093</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1427,15 +1404,15 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1451,7 +1428,7 @@
         <v>6127</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1498,15 +1475,15 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1522,7 +1499,7 @@
         <v>8191</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1536,7 +1513,7 @@
     </row>
     <row r="34" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M34" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1574,15 +1551,15 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1598,12 +1575,12 @@
         <v>1586</v>
       </c>
       <c r="F2" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <f>B4-E3</f>
@@ -1620,12 +1597,12 @@
         <v>186</v>
       </c>
       <c r="F3" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B4">
         <f>8192-E4</f>
@@ -1642,7 +1619,7 @@
         <v>35</v>
       </c>
       <c r="F4" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1692,24 +1669,24 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="G1" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="H1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="I1" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1739,7 +1716,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B3">
         <f>G2+1</f>
@@ -1770,7 +1747,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B4">
         <f>G3+1</f>
@@ -1841,24 +1818,24 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1888,7 +1865,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B3">
         <f>G2+1</f>
@@ -1933,9 +1910,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8A806B9-8F96-4CFC-8F80-C6046C4BB66C}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1945,144 +1920,98 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="A1" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>185</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <f>C2*D2</f>
-        <v>185</v>
-      </c>
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3">
-        <f>B2+ E2+1</f>
-        <v>186</v>
-      </c>
-      <c r="C3">
-        <v>5</v>
-      </c>
-      <c r="D3">
-        <v>255</v>
-      </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E6" si="0">C3*D3</f>
-        <v>1275</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4">
-        <f>B3+ E3+1</f>
-        <v>1462</v>
-      </c>
-      <c r="C4">
-        <v>5</v>
-      </c>
-      <c r="D4">
-        <v>255</v>
-      </c>
-      <c r="E4">
-        <f t="shared" si="0"/>
-        <v>1275</v>
-      </c>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5">
-        <f>B4+ E4+1</f>
-        <v>2738</v>
-      </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-      <c r="D5">
-        <v>255</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="0"/>
-        <v>1275</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6">
-        <f>B5+ E5+1</f>
-        <v>4014</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-      <c r="D6">
-        <v>255</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="0"/>
-        <v>1275</v>
-      </c>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9">
-        <f>BANK0x3E!B4+ BANK0x3E!E4+1</f>
-        <v>5874</v>
-      </c>
-      <c r="C9">
-        <v>10</v>
-      </c>
-      <c r="D9">
-        <v>20</v>
-      </c>
-      <c r="E9">
-        <f t="shared" ref="E9" si="1">C9*D9</f>
-        <v>200</v>
-      </c>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13">
-        <f>SUM(E2:E11)</f>
-        <v>5485</v>
-      </c>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2094,9 +2023,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A86A6CAE-A2FB-4700-AF3B-F451BF94FBFE}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2106,112 +2033,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="A1" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>9</v>
-      </c>
-      <c r="D2">
-        <v>20</v>
-      </c>
-      <c r="E2">
-        <f t="shared" ref="E2" si="0">C2*D2</f>
-        <v>180</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3">
-        <f>B2+ E2+1</f>
-        <v>181</v>
-      </c>
-      <c r="C3">
-        <v>9</v>
-      </c>
-      <c r="D3">
-        <f>D2*20</f>
-        <v>400</v>
-      </c>
-      <c r="E3">
-        <f t="shared" ref="E3" si="1">C3*D3</f>
-        <v>3600</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4">
-        <f>B3+ E3+1</f>
-        <v>3782</v>
-      </c>
-      <c r="C4">
-        <v>42</v>
-      </c>
-      <c r="D4">
-        <v>20</v>
-      </c>
-      <c r="E4">
-        <f t="shared" ref="E4" si="2">C4*D4</f>
-        <v>840</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5">
-        <f>B4+ E4+1</f>
-        <v>4623</v>
-      </c>
-      <c r="C5">
-        <v>12</v>
-      </c>
-      <c r="D5">
-        <v>256</v>
-      </c>
-      <c r="E5">
-        <f t="shared" ref="E5" si="3">C5*D5</f>
-        <v>3072</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>46</v>
-      </c>
-    </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13">
-        <f>SUM(E2:E11)</f>
-        <v>7692</v>
-      </c>
+      <c r="A13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2248,13 +2080,13 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -2272,7 +2104,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <f>E2 + 1</f>
@@ -2291,7 +2123,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B4">
         <f>B3+ E3+1</f>
@@ -2310,7 +2142,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -2356,15 +2188,15 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -2386,7 +2218,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B3">
         <f>B2+ E2+1</f>
@@ -2409,7 +2241,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B4">
         <f>B3+ E3+1</f>
@@ -2432,7 +2264,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B5">
         <f>B4+ E4+1</f>
@@ -2455,12 +2287,12 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E10">
         <f>SUM(E2:E9)</f>
@@ -2469,7 +2301,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E11">
         <v>1023</v>
@@ -2512,27 +2344,27 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -2565,7 +2397,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B3">
         <f>C2</f>
@@ -2599,7 +2431,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="B4">
         <f t="shared" ref="B4:B6" si="3">B3+C3</f>
@@ -2633,7 +2465,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B5">
         <f t="shared" si="3"/>
@@ -2667,7 +2499,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B6">
         <f t="shared" si="3"/>
@@ -2687,7 +2519,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B7">
         <f t="shared" ref="B7" si="4">B6+C6</f>
@@ -2707,7 +2539,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="C9">
         <f>C7+C4</f>
@@ -2716,7 +2548,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C10">
         <f>SUM(C2:C7)</f>
@@ -2725,7 +2557,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C11">
         <v>129471</v>
@@ -2733,7 +2565,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C12">
         <f>C11-C10</f>
@@ -2789,21 +2621,21 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -2819,7 +2651,7 @@
         <v>7470</v>
       </c>
       <c r="F2" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="G2" t="str">
         <f>DEC2HEX(HEX2DEC("A000"))</f>
@@ -2832,7 +2664,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B3">
         <f>C2</f>
@@ -2859,7 +2691,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B4">
         <f>B3+E3</f>
@@ -2892,7 +2724,7 @@
     <row r="6" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="7" spans="1:8" ht="253" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
@@ -2940,15 +2772,15 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -2964,7 +2796,7 @@
         <v>8191</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -3012,15 +2844,15 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -3036,7 +2868,7 @@
         <v>8191</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -3084,24 +2916,24 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="G1" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="H1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="I1" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -3131,26 +2963,26 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -3164,7 +2996,7 @@
     </row>
     <row r="13" spans="1:9" ht="145" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -3202,15 +3034,15 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -3226,7 +3058,7 @@
         <v>8191</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -3273,15 +3105,15 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -3297,7 +3129,7 @@
         <v>6696</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Revert "Moved loadedPictures to bss for easy allocation and to free up the bank"
This reverts commit 5a7820efc3e5dabdcf073aa996447e5be60fa158.
</commit_message>
<xml_diff>
--- a/docs/allocation.xlsx
+++ b/docs/allocation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD63415F-EE79-45DE-9581-D2927FFC47D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC068A5-9723-4E61-933F-AAC00EF84FEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" firstSheet="8" activeTab="21" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic (Bank 0x13 - 0x26)" sheetId="2" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="86">
   <si>
     <t>Type</t>
   </si>
@@ -104,6 +104,21 @@
     <t>Start</t>
   </si>
   <si>
+    <t>Allocation Array</t>
+  </si>
+  <si>
+    <t>logDir</t>
+  </si>
+  <si>
+    <t>picDir</t>
+  </si>
+  <si>
+    <t>soundDir</t>
+  </si>
+  <si>
+    <t>viewDir</t>
+  </si>
+  <si>
     <t>logicEntry</t>
   </si>
   <si>
@@ -128,6 +143,12 @@
     <t>workArea</t>
   </si>
   <si>
+    <t>menu</t>
+  </si>
+  <si>
+    <t>menuChild</t>
+  </si>
+  <si>
     <t>code</t>
   </si>
   <si>
@@ -138,6 +159,12 @@
   </si>
   <si>
     <t>getNumTemp</t>
+  </si>
+  <si>
+    <t>viewTab</t>
+  </si>
+  <si>
+    <t>loadedView</t>
   </si>
   <si>
     <t>TBD</t>
@@ -296,9 +323,6 @@
   </si>
   <si>
     <t>Sprites Small</t>
-  </si>
-  <si>
-    <t>vacant</t>
   </si>
 </sst>
 </file>
@@ -342,14 +366,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -666,7 +689,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{355DE0EA-5B2C-4635-84EE-7D1B81ED29C7}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
@@ -722,7 +745,7 @@
         <v>8000</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -749,7 +772,7 @@
         <v>8000</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="F3">
         <f>D3/8000</f>
@@ -779,7 +802,7 @@
         <v>48000</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F4">
         <v>6</v>
@@ -808,7 +831,7 @@
         <v>48000</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="F5">
         <v>6</v>
@@ -837,7 +860,7 @@
         <v>48000</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="F6">
         <f>D6/8000</f>
@@ -909,15 +932,15 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -932,7 +955,7 @@
         <v>8191</v>
       </c>
       <c r="F2" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -979,15 +1002,15 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1003,7 +1026,7 @@
         <v>8191</v>
       </c>
       <c r="F2" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1050,15 +1073,15 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1074,7 +1097,7 @@
         <v>8191</v>
       </c>
       <c r="F2" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1121,15 +1144,15 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1145,7 +1168,7 @@
         <v>3586</v>
       </c>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1192,15 +1215,15 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1216,7 +1239,7 @@
         <v>5123</v>
       </c>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1263,15 +1286,15 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1287,7 +1310,7 @@
         <v>3723</v>
       </c>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1334,15 +1357,15 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1357,7 +1380,7 @@
         <v>3093</v>
       </c>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1404,15 +1427,15 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1428,7 +1451,7 @@
         <v>6127</v>
       </c>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1475,15 +1498,15 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1499,7 +1522,7 @@
         <v>8191</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1513,7 +1536,7 @@
     </row>
     <row r="34" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M34" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1551,15 +1574,15 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1575,12 +1598,12 @@
         <v>1586</v>
       </c>
       <c r="F2" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B3">
         <f>B4-E3</f>
@@ -1597,12 +1620,12 @@
         <v>186</v>
       </c>
       <c r="F3" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B4">
         <f>8192-E4</f>
@@ -1619,7 +1642,7 @@
         <v>35</v>
       </c>
       <c r="F4" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1669,24 +1692,24 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F1" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="G1" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="H1" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="I1" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1716,7 +1739,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="B3">
         <f>G2+1</f>
@@ -1747,7 +1770,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="B4">
         <f>G3+1</f>
@@ -1818,24 +1841,24 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1865,7 +1888,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="B3">
         <f>G2+1</f>
@@ -1910,7 +1933,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8A806B9-8F96-4CFC-8F80-C6046C4BB66C}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1920,98 +1945,144 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>185</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f>C2*D2</f>
+        <v>185</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3">
+        <f>B2+ E2+1</f>
+        <v>186</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>255</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E6" si="0">C3*D3</f>
+        <v>1275</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4">
+        <f>B3+ E3+1</f>
+        <v>1462</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>255</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>1275</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5">
+        <f>B4+ E4+1</f>
+        <v>2738</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>255</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>1275</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6">
+        <f>B5+ E5+1</f>
+        <v>4014</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>255</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>1275</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9">
+        <f>BANK0x3E!B4+ BANK0x3E!E4+1</f>
+        <v>5874</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>20</v>
+      </c>
+      <c r="E9">
+        <f t="shared" ref="E9" si="1">C9*D9</f>
+        <v>200</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <f>SUM(E2:E11)</f>
+        <v>5485</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2023,7 +2094,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A86A6CAE-A2FB-4700-AF3B-F451BF94FBFE}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2033,17 +2106,112 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="F1" s="1"/>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <v>20</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ref="E2" si="0">C2*D2</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3">
+        <f>B2+ E2+1</f>
+        <v>181</v>
+      </c>
+      <c r="C3">
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <f>D2*20</f>
+        <v>400</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3" si="1">C3*D3</f>
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4">
+        <f>B3+ E3+1</f>
+        <v>3782</v>
+      </c>
+      <c r="C4">
+        <v>42</v>
+      </c>
+      <c r="D4">
+        <v>20</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4" si="2">C4*D4</f>
+        <v>840</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5">
+        <f>B4+ E4+1</f>
+        <v>4623</v>
+      </c>
+      <c r="C5">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>256</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ref="E5" si="3">C5*D5</f>
+        <v>3072</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+    </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <f>SUM(E2:E11)</f>
+        <v>7692</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2080,13 +2248,13 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -2104,7 +2272,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B3">
         <f>E2 + 1</f>
@@ -2123,7 +2291,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B4">
         <f>B3+ E3+1</f>
@@ -2142,7 +2310,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -2188,15 +2356,15 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -2218,7 +2386,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B3">
         <f>B2+ E2+1</f>
@@ -2241,7 +2409,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B4">
         <f>B3+ E3+1</f>
@@ -2264,7 +2432,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="B5">
         <f>B4+ E4+1</f>
@@ -2287,12 +2455,12 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E10">
         <f>SUM(E2:E9)</f>
@@ -2301,7 +2469,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E11">
         <v>1023</v>
@@ -2344,27 +2512,27 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -2397,7 +2565,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="B3">
         <f>C2</f>
@@ -2431,7 +2599,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="B4">
         <f t="shared" ref="B4:B6" si="3">B3+C3</f>
@@ -2465,7 +2633,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="B5">
         <f t="shared" si="3"/>
@@ -2499,7 +2667,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="B6">
         <f t="shared" si="3"/>
@@ -2519,7 +2687,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="B7">
         <f t="shared" ref="B7" si="4">B6+C6</f>
@@ -2539,7 +2707,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="C9">
         <f>C7+C4</f>
@@ -2548,7 +2716,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="C10">
         <f>SUM(C2:C7)</f>
@@ -2557,7 +2725,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="C11">
         <v>129471</v>
@@ -2565,7 +2733,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="C12">
         <f>C11-C10</f>
@@ -2621,21 +2789,21 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -2651,7 +2819,7 @@
         <v>7470</v>
       </c>
       <c r="F2" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="G2" t="str">
         <f>DEC2HEX(HEX2DEC("A000"))</f>
@@ -2664,7 +2832,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="B3">
         <f>C2</f>
@@ -2691,7 +2859,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="B4">
         <f>B3+E3</f>
@@ -2724,7 +2892,7 @@
     <row r="6" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="7" spans="1:8" ht="253" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
@@ -2772,15 +2940,15 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -2796,7 +2964,7 @@
         <v>8191</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -2844,15 +3012,15 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -2868,7 +3036,7 @@
         <v>8191</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -2916,24 +3084,24 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F1" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="G1" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="H1" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="I1" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -2963,26 +3131,26 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -2996,7 +3164,7 @@
     </row>
     <row r="13" spans="1:9" ht="145" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -3034,15 +3202,15 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -3058,7 +3226,7 @@
         <v>8191</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -3105,15 +3273,15 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -3129,7 +3297,7 @@
         <v>6696</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Clearing priority screen on clear
</commit_message>
<xml_diff>
--- a/docs/allocation.xlsx
+++ b/docs/allocation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC068A5-9723-4E61-933F-AAC00EF84FEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{239A6168-EE85-4944-A2DD-338A2A37B96E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" firstSheet="9" activeTab="24" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic (Bank 0x13 - 0x26)" sheetId="2" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="82">
   <si>
     <t>Type</t>
   </si>
@@ -305,18 +305,6 @@
   </si>
   <si>
     <t>code/buffers</t>
-  </si>
-  <si>
-    <t>No Sprites</t>
-  </si>
-  <si>
-    <t>Sprite Width</t>
-  </si>
-  <si>
-    <t>Average Loop Length</t>
-  </si>
-  <si>
-    <t>Average Loop limit</t>
   </si>
   <si>
     <t>Available For Sprites</t>
@@ -689,7 +677,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{355DE0EA-5B2C-4635-84EE-7D1B81ED29C7}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
@@ -2483,10 +2471,10 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C9D07F7-AEFD-4D2F-97E3-087A93BF23D8}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2517,18 +2505,10 @@
       <c r="E1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>83</v>
-      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -2545,22 +2525,8 @@
         <v>0</v>
       </c>
       <c r="E2" t="str">
-        <f t="shared" ref="E2:E6" si="0">DEC2HEX(HEX2DEC(D2)+C2-1)</f>
+        <f t="shared" ref="E2:E7" si="0">DEC2HEX(HEX2DEC(D2)+C2-1)</f>
         <v>95FF</v>
-      </c>
-      <c r="F2">
-        <f>C4/((G2*G2)/2)</f>
-        <v>46.5</v>
-      </c>
-      <c r="G2">
-        <v>8</v>
-      </c>
-      <c r="H2">
-        <v>7</v>
-      </c>
-      <c r="I2">
-        <f>F2/H2</f>
-        <v>6.6428571428571432</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -2572,171 +2538,149 @@
         <v>38400</v>
       </c>
       <c r="C3">
-        <v>13360</v>
+        <v>13440</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D6" si="1">DEC2HEX(B2 + C2)</f>
+        <f t="shared" ref="D3:D7" si="1">DEC2HEX(B2 + C2)</f>
         <v>9600</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" si="0"/>
-        <v>CA2F</v>
-      </c>
-      <c r="F3">
-        <f>C4/((G3*G3)/2)</f>
-        <v>11.625</v>
-      </c>
-      <c r="G3">
-        <v>16</v>
-      </c>
-      <c r="H3">
-        <v>7</v>
-      </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I5" si="2">F3/H3</f>
-        <v>1.6607142857142858</v>
+        <v>CA7F</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B6" si="3">B3+C3</f>
-        <v>51760</v>
+        <f>B3+ C3</f>
+        <v>51840</v>
       </c>
       <c r="C4">
-        <v>1488</v>
+        <v>128</v>
       </c>
       <c r="D4" t="str">
-        <f t="shared" si="1"/>
-        <v>CA30</v>
+        <f t="shared" ref="D4" si="2">DEC2HEX(B3 + C3)</f>
+        <v>CA80</v>
       </c>
       <c r="E4" t="str">
+        <f t="shared" ref="E4" si="3">DEC2HEX(HEX2DEC(D4)+C4-1)</f>
+        <v>CAFF</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5">
+        <f>B4+C4</f>
+        <v>51968</v>
+      </c>
+      <c r="C5">
+        <v>1280</v>
+      </c>
+      <c r="D5" t="str">
+        <f>DEC2HEX(B4 + C4)</f>
+        <v>CB00</v>
+      </c>
+      <c r="E5" t="str">
         <f t="shared" si="0"/>
         <v>CFFF</v>
       </c>
-      <c r="F4">
-        <f>C7/((G4*G4)/2)</f>
-        <v>135</v>
-      </c>
-      <c r="G4">
-        <v>32</v>
-      </c>
-      <c r="H4">
-        <v>7</v>
-      </c>
-      <c r="I4">
-        <f t="shared" si="2"/>
-        <v>19.285714285714285</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>72</v>
       </c>
-      <c r="B5">
-        <f t="shared" si="3"/>
+      <c r="B6">
+        <f t="shared" ref="B6:B8" si="4">B5+C5</f>
         <v>53248</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <v>2560</v>
       </c>
-      <c r="D5" t="str">
+      <c r="D6" t="str">
         <f t="shared" si="1"/>
         <v>D000</v>
       </c>
-      <c r="E5" t="str">
+      <c r="E6" t="str">
         <f t="shared" si="0"/>
         <v>D9FF</v>
       </c>
-      <c r="F5">
-        <f>C7/((G5*G5)/2)</f>
-        <v>33.75</v>
-      </c>
-      <c r="G5">
-        <v>64</v>
-      </c>
-      <c r="H5">
-        <v>7</v>
-      </c>
-      <c r="I5">
-        <f t="shared" si="2"/>
-        <v>4.8214285714285712</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>73</v>
       </c>
-      <c r="B6">
-        <f t="shared" si="3"/>
+      <c r="B7">
+        <f t="shared" si="4"/>
         <v>55808</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <v>4096</v>
       </c>
-      <c r="D6" t="str">
+      <c r="D7" t="str">
         <f t="shared" si="1"/>
         <v>DA00</v>
       </c>
-      <c r="E6" t="str">
+      <c r="E7" t="str">
         <f t="shared" si="0"/>
         <v>E9FF</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>77</v>
       </c>
-      <c r="B7">
-        <f t="shared" ref="B7" si="4">B6+C6</f>
+      <c r="B8">
+        <f t="shared" si="4"/>
         <v>59904</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>69120</v>
       </c>
-      <c r="D7" t="str">
-        <f t="shared" ref="D7" si="5">DEC2HEX(B6 + C6)</f>
+      <c r="D8" t="str">
+        <f t="shared" ref="D8" si="5">DEC2HEX(B7 + C7)</f>
         <v>EA00</v>
       </c>
-      <c r="E7" t="str">
-        <f t="shared" ref="E7" si="6">DEC2HEX(HEX2DEC(D7)+C7-1)</f>
+      <c r="E8" t="str">
+        <f t="shared" ref="E8" si="6">DEC2HEX(HEX2DEC(D8)+C8-1)</f>
         <v>1F7FF</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B9" t="s">
-        <v>84</v>
-      </c>
-      <c r="C9">
-        <f>C7+C4</f>
-        <v>70608</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="C10">
-        <f>SUM(C2:C7)</f>
-        <v>129024</v>
+        <f>C8+C5</f>
+        <v>70400</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C11">
-        <v>129471</v>
+        <f>SUM(C2:C8)</f>
+        <v>129024</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12">
+        <v>129471</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
         <v>76</v>
       </c>
-      <c r="C12">
-        <f>C11-C10</f>
+      <c r="C13">
+        <f>C12-C11</f>
         <v>447</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Successfully moved sprite garbage collection mechanism to bank C, as E was full
</commit_message>
<xml_diff>
--- a/docs/allocation.xlsx
+++ b/docs/allocation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{239A6168-EE85-4944-A2DD-338A2A37B96E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E53819-EF13-4656-9259-5A52F4540A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" firstSheet="9" activeTab="24" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" firstSheet="10" activeTab="25" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic (Bank 0x13 - 0x26)" sheetId="2" r:id="rId1"/>
@@ -38,6 +38,7 @@
     <sheet name="BANK0x3E" sheetId="20" r:id="rId23"/>
     <sheet name="Golden" sheetId="4" r:id="rId24"/>
     <sheet name="Vera" sheetId="27" r:id="rId25"/>
+    <sheet name="Sprite Addresses" sheetId="28" r:id="rId26"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="220">
   <si>
     <t>Type</t>
   </si>
@@ -311,6 +312,420 @@
   </si>
   <si>
     <t>Sprites Small</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>0XEA00</t>
+  </si>
+  <si>
+    <t>0XEC00</t>
+  </si>
+  <si>
+    <t>0XEE00</t>
+  </si>
+  <si>
+    <t>0XF000</t>
+  </si>
+  <si>
+    <t>0XF200</t>
+  </si>
+  <si>
+    <t>0XF400</t>
+  </si>
+  <si>
+    <t>0XF600</t>
+  </si>
+  <si>
+    <t>0XF800</t>
+  </si>
+  <si>
+    <t>0XFA00</t>
+  </si>
+  <si>
+    <t>0XFC00</t>
+  </si>
+  <si>
+    <t>0XFE00</t>
+  </si>
+  <si>
+    <t>0X10000</t>
+  </si>
+  <si>
+    <t>0X10200</t>
+  </si>
+  <si>
+    <t>0X10400</t>
+  </si>
+  <si>
+    <t>0X10600</t>
+  </si>
+  <si>
+    <t>0X10800</t>
+  </si>
+  <si>
+    <t>0X10A00</t>
+  </si>
+  <si>
+    <t>0X10C00</t>
+  </si>
+  <si>
+    <t>0X10E00</t>
+  </si>
+  <si>
+    <t>0X11000</t>
+  </si>
+  <si>
+    <t>0X11200</t>
+  </si>
+  <si>
+    <t>0X11400</t>
+  </si>
+  <si>
+    <t>0X11600</t>
+  </si>
+  <si>
+    <t>0X11800</t>
+  </si>
+  <si>
+    <t>0X11A00</t>
+  </si>
+  <si>
+    <t>0X11C00</t>
+  </si>
+  <si>
+    <t>0X11E00</t>
+  </si>
+  <si>
+    <t>0X12000</t>
+  </si>
+  <si>
+    <t>0X12200</t>
+  </si>
+  <si>
+    <t>0X12400</t>
+  </si>
+  <si>
+    <t>0X12600</t>
+  </si>
+  <si>
+    <t>0X12800</t>
+  </si>
+  <si>
+    <t>0X12A00</t>
+  </si>
+  <si>
+    <t>0X12C00</t>
+  </si>
+  <si>
+    <t>0X12E00</t>
+  </si>
+  <si>
+    <t>0X13000</t>
+  </si>
+  <si>
+    <t>0X13200</t>
+  </si>
+  <si>
+    <t>0X13400</t>
+  </si>
+  <si>
+    <t>0X13600</t>
+  </si>
+  <si>
+    <t>0X13800</t>
+  </si>
+  <si>
+    <t>0X13A00</t>
+  </si>
+  <si>
+    <t>0X13C00</t>
+  </si>
+  <si>
+    <t>0X13E00</t>
+  </si>
+  <si>
+    <t>0X14000</t>
+  </si>
+  <si>
+    <t>0X14200</t>
+  </si>
+  <si>
+    <t>0X14400</t>
+  </si>
+  <si>
+    <t>0X14600</t>
+  </si>
+  <si>
+    <t>0X14800</t>
+  </si>
+  <si>
+    <t>0X14A00</t>
+  </si>
+  <si>
+    <t>0X14C00</t>
+  </si>
+  <si>
+    <t>0X14E00</t>
+  </si>
+  <si>
+    <t>0X15000</t>
+  </si>
+  <si>
+    <t>0X15200</t>
+  </si>
+  <si>
+    <t>0X15400</t>
+  </si>
+  <si>
+    <t>0X15600</t>
+  </si>
+  <si>
+    <t>0X15800</t>
+  </si>
+  <si>
+    <t>0X15A00</t>
+  </si>
+  <si>
+    <t>0X15C00</t>
+  </si>
+  <si>
+    <t>0X15E00</t>
+  </si>
+  <si>
+    <t>0X16000</t>
+  </si>
+  <si>
+    <t>0X16200</t>
+  </si>
+  <si>
+    <t>0X16400</t>
+  </si>
+  <si>
+    <t>0X16600</t>
+  </si>
+  <si>
+    <t>0X16800</t>
+  </si>
+  <si>
+    <t>0X16A00</t>
+  </si>
+  <si>
+    <t>0X16C00</t>
+  </si>
+  <si>
+    <t>0X16E00</t>
+  </si>
+  <si>
+    <t>0X17000</t>
+  </si>
+  <si>
+    <t>0X17200</t>
+  </si>
+  <si>
+    <t>0X17400</t>
+  </si>
+  <si>
+    <t>0X17600</t>
+  </si>
+  <si>
+    <t>0X17800</t>
+  </si>
+  <si>
+    <t>0X17A00</t>
+  </si>
+  <si>
+    <t>0X17C00</t>
+  </si>
+  <si>
+    <t>0X17E00</t>
+  </si>
+  <si>
+    <t>0X18000</t>
+  </si>
+  <si>
+    <t>0X18200</t>
+  </si>
+  <si>
+    <t>0X18400</t>
+  </si>
+  <si>
+    <t>0X18600</t>
+  </si>
+  <si>
+    <t>0X18800</t>
+  </si>
+  <si>
+    <t>0X18A00</t>
+  </si>
+  <si>
+    <t>0X18C00</t>
+  </si>
+  <si>
+    <t>0X18E00</t>
+  </si>
+  <si>
+    <t>0X19000</t>
+  </si>
+  <si>
+    <t>0X19200</t>
+  </si>
+  <si>
+    <t>0X19400</t>
+  </si>
+  <si>
+    <t>0X19600</t>
+  </si>
+  <si>
+    <t>0X19800</t>
+  </si>
+  <si>
+    <t>0X19A00</t>
+  </si>
+  <si>
+    <t>0X19C00</t>
+  </si>
+  <si>
+    <t>0X19E00</t>
+  </si>
+  <si>
+    <t>0X1A000</t>
+  </si>
+  <si>
+    <t>0X1A200</t>
+  </si>
+  <si>
+    <t>0X1A400</t>
+  </si>
+  <si>
+    <t>0X1A600</t>
+  </si>
+  <si>
+    <t>0X1A800</t>
+  </si>
+  <si>
+    <t>0X1AA00</t>
+  </si>
+  <si>
+    <t>0X1AC00</t>
+  </si>
+  <si>
+    <t>0X1AE00</t>
+  </si>
+  <si>
+    <t>0X1B000</t>
+  </si>
+  <si>
+    <t>0X1B200</t>
+  </si>
+  <si>
+    <t>0X1B400</t>
+  </si>
+  <si>
+    <t>0X1B600</t>
+  </si>
+  <si>
+    <t>0X1B800</t>
+  </si>
+  <si>
+    <t>0X1BA00</t>
+  </si>
+  <si>
+    <t>0X1BC00</t>
+  </si>
+  <si>
+    <t>0X1BE00</t>
+  </si>
+  <si>
+    <t>0X1C000</t>
+  </si>
+  <si>
+    <t>0X1C200</t>
+  </si>
+  <si>
+    <t>0X1C400</t>
+  </si>
+  <si>
+    <t>0X1C600</t>
+  </si>
+  <si>
+    <t>0X1C800</t>
+  </si>
+  <si>
+    <t>0X1CA00</t>
+  </si>
+  <si>
+    <t>0X1CC00</t>
+  </si>
+  <si>
+    <t>0X1CE00</t>
+  </si>
+  <si>
+    <t>0X1D000</t>
+  </si>
+  <si>
+    <t>0X1D200</t>
+  </si>
+  <si>
+    <t>0X1D400</t>
+  </si>
+  <si>
+    <t>0X1D600</t>
+  </si>
+  <si>
+    <t>0X1D800</t>
+  </si>
+  <si>
+    <t>0X1DA00</t>
+  </si>
+  <si>
+    <t>0X1DC00</t>
+  </si>
+  <si>
+    <t>0X1DE00</t>
+  </si>
+  <si>
+    <t>0X1E000</t>
+  </si>
+  <si>
+    <t>0X1E200</t>
+  </si>
+  <si>
+    <t>0X1E400</t>
+  </si>
+  <si>
+    <t>0X1E600</t>
+  </si>
+  <si>
+    <t>0X1E800</t>
+  </si>
+  <si>
+    <t>0X1EA00</t>
+  </si>
+  <si>
+    <t>0X1EC00</t>
+  </si>
+  <si>
+    <t>0X1EE00</t>
+  </si>
+  <si>
+    <t>0X1F000</t>
+  </si>
+  <si>
+    <t>0X1F200</t>
+  </si>
+  <si>
+    <t>0X1F400</t>
+  </si>
+  <si>
+    <t>0X1F600</t>
+  </si>
+  <si>
+    <t>All possible sprite addresses and their index in _bESpriteAllocTable</t>
   </si>
 </sst>
 </file>
@@ -2473,7 +2888,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C9D07F7-AEFD-4D2F-97E3-087A93BF23D8}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -2687,6 +3102,1115 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72D5F9F0-2373-44BA-8150-CDB117860CA2}">
+  <dimension ref="A1:D136"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="119.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>47</v>
+      </c>
+      <c r="B49" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>48</v>
+      </c>
+      <c r="B50" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>49</v>
+      </c>
+      <c r="B51" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>50</v>
+      </c>
+      <c r="B52" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>51</v>
+      </c>
+      <c r="B53" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>52</v>
+      </c>
+      <c r="B54" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <v>53</v>
+      </c>
+      <c r="B55" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56">
+        <v>54</v>
+      </c>
+      <c r="B56" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <v>55</v>
+      </c>
+      <c r="B57" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A58">
+        <v>56</v>
+      </c>
+      <c r="B58" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <v>57</v>
+      </c>
+      <c r="B59" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A60">
+        <v>58</v>
+      </c>
+      <c r="B60" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A61">
+        <v>59</v>
+      </c>
+      <c r="B61" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A62">
+        <v>60</v>
+      </c>
+      <c r="B62" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A63">
+        <v>61</v>
+      </c>
+      <c r="B63" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A64">
+        <v>62</v>
+      </c>
+      <c r="B64" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A65">
+        <v>63</v>
+      </c>
+      <c r="B65" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A66">
+        <v>64</v>
+      </c>
+      <c r="B66" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A67">
+        <v>65</v>
+      </c>
+      <c r="B67" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A68">
+        <v>66</v>
+      </c>
+      <c r="B68" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A69">
+        <v>67</v>
+      </c>
+      <c r="B69" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A70">
+        <v>68</v>
+      </c>
+      <c r="B70" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A71">
+        <v>69</v>
+      </c>
+      <c r="B71" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A72">
+        <v>70</v>
+      </c>
+      <c r="B72" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A73">
+        <v>71</v>
+      </c>
+      <c r="B73" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A74">
+        <v>72</v>
+      </c>
+      <c r="B74" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A75">
+        <v>73</v>
+      </c>
+      <c r="B75" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A76">
+        <v>74</v>
+      </c>
+      <c r="B76" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A77">
+        <v>75</v>
+      </c>
+      <c r="B77" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A78">
+        <v>76</v>
+      </c>
+      <c r="B78" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A79">
+        <v>77</v>
+      </c>
+      <c r="B79" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A80">
+        <v>78</v>
+      </c>
+      <c r="B80" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A81">
+        <v>79</v>
+      </c>
+      <c r="B81" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A82">
+        <v>80</v>
+      </c>
+      <c r="B82" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A83">
+        <v>81</v>
+      </c>
+      <c r="B83" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A84">
+        <v>82</v>
+      </c>
+      <c r="B84" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A85">
+        <v>83</v>
+      </c>
+      <c r="B85" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A86">
+        <v>84</v>
+      </c>
+      <c r="B86" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A87">
+        <v>85</v>
+      </c>
+      <c r="B87" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A88">
+        <v>86</v>
+      </c>
+      <c r="B88" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A89">
+        <v>87</v>
+      </c>
+      <c r="B89" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A90">
+        <v>88</v>
+      </c>
+      <c r="B90" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A91">
+        <v>89</v>
+      </c>
+      <c r="B91" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A92">
+        <v>90</v>
+      </c>
+      <c r="B92" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A93">
+        <v>91</v>
+      </c>
+      <c r="B93" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A94">
+        <v>92</v>
+      </c>
+      <c r="B94" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A95">
+        <v>93</v>
+      </c>
+      <c r="B95" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A96">
+        <v>94</v>
+      </c>
+      <c r="B96" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A97">
+        <v>95</v>
+      </c>
+      <c r="B97" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A98">
+        <v>96</v>
+      </c>
+      <c r="B98" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A99">
+        <v>97</v>
+      </c>
+      <c r="B99" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A100">
+        <v>98</v>
+      </c>
+      <c r="B100" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A101">
+        <v>99</v>
+      </c>
+      <c r="B101" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A102">
+        <v>100</v>
+      </c>
+      <c r="B102" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A103">
+        <v>101</v>
+      </c>
+      <c r="B103" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A104">
+        <v>102</v>
+      </c>
+      <c r="B104" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A105">
+        <v>103</v>
+      </c>
+      <c r="B105" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A106">
+        <v>104</v>
+      </c>
+      <c r="B106" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A107">
+        <v>105</v>
+      </c>
+      <c r="B107" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A108">
+        <v>106</v>
+      </c>
+      <c r="B108" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A109">
+        <v>107</v>
+      </c>
+      <c r="B109" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A110">
+        <v>108</v>
+      </c>
+      <c r="B110" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A111">
+        <v>109</v>
+      </c>
+      <c r="B111" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A112">
+        <v>110</v>
+      </c>
+      <c r="B112" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A113">
+        <v>111</v>
+      </c>
+      <c r="B113" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A114">
+        <v>112</v>
+      </c>
+      <c r="B114" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A115">
+        <v>113</v>
+      </c>
+      <c r="B115" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A116">
+        <v>114</v>
+      </c>
+      <c r="B116" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A117">
+        <v>115</v>
+      </c>
+      <c r="B117" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A118">
+        <v>116</v>
+      </c>
+      <c r="B118" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A119">
+        <v>117</v>
+      </c>
+      <c r="B119" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A120">
+        <v>118</v>
+      </c>
+      <c r="B120" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A121">
+        <v>119</v>
+      </c>
+      <c r="B121" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A122">
+        <v>120</v>
+      </c>
+      <c r="B122" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A123">
+        <v>121</v>
+      </c>
+      <c r="B123" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A124">
+        <v>122</v>
+      </c>
+      <c r="B124" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A125">
+        <v>123</v>
+      </c>
+      <c r="B125" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A126">
+        <v>124</v>
+      </c>
+      <c r="B126" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A127">
+        <v>125</v>
+      </c>
+      <c r="B127" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A128">
+        <v>126</v>
+      </c>
+      <c r="B128" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A129">
+        <v>127</v>
+      </c>
+      <c r="B129" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A130">
+        <v>128</v>
+      </c>
+      <c r="B130" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A131">
+        <v>129</v>
+      </c>
+      <c r="B131" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A132">
+        <v>130</v>
+      </c>
+      <c r="B132" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A133">
+        <v>131</v>
+      </c>
+      <c r="B133" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A134">
+        <v>132</v>
+      </c>
+      <c r="B134" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A135">
+        <v>133</v>
+      </c>
+      <c r="B135" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A136">
+        <v>134</v>
+      </c>
+      <c r="B136" t="s">
+        <v>218</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Moved loaded view to bank 11 meaning that its position is automatically calculated
</commit_message>
<xml_diff>
--- a/docs/allocation.xlsx
+++ b/docs/allocation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{239A6168-EE85-4944-A2DD-338A2A37B96E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C236F3-A4CF-4EED-B259-9AA57D680C91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" firstSheet="9" activeTab="24" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" firstSheet="12" activeTab="20" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic (Bank 0x13 - 0x26)" sheetId="2" r:id="rId1"/>
@@ -38,6 +38,7 @@
     <sheet name="BANK0x3E" sheetId="20" r:id="rId23"/>
     <sheet name="Golden" sheetId="4" r:id="rId24"/>
     <sheet name="Vera" sheetId="27" r:id="rId25"/>
+    <sheet name="Sprite Addresses" sheetId="28" r:id="rId26"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="218">
   <si>
     <t>Type</t>
   </si>
@@ -159,12 +160,6 @@
   </si>
   <si>
     <t>getNumTemp</t>
-  </si>
-  <si>
-    <t>viewTab</t>
-  </si>
-  <si>
-    <t>loadedView</t>
   </si>
   <si>
     <t>TBD</t>
@@ -311,6 +306,420 @@
   </si>
   <si>
     <t>Sprites Small</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>0XEA00</t>
+  </si>
+  <si>
+    <t>0XEC00</t>
+  </si>
+  <si>
+    <t>0XEE00</t>
+  </si>
+  <si>
+    <t>0XF000</t>
+  </si>
+  <si>
+    <t>0XF200</t>
+  </si>
+  <si>
+    <t>0XF400</t>
+  </si>
+  <si>
+    <t>0XF600</t>
+  </si>
+  <si>
+    <t>0XF800</t>
+  </si>
+  <si>
+    <t>0XFA00</t>
+  </si>
+  <si>
+    <t>0XFC00</t>
+  </si>
+  <si>
+    <t>0XFE00</t>
+  </si>
+  <si>
+    <t>0X10000</t>
+  </si>
+  <si>
+    <t>0X10200</t>
+  </si>
+  <si>
+    <t>0X10400</t>
+  </si>
+  <si>
+    <t>0X10600</t>
+  </si>
+  <si>
+    <t>0X10800</t>
+  </si>
+  <si>
+    <t>0X10A00</t>
+  </si>
+  <si>
+    <t>0X10C00</t>
+  </si>
+  <si>
+    <t>0X10E00</t>
+  </si>
+  <si>
+    <t>0X11000</t>
+  </si>
+  <si>
+    <t>0X11200</t>
+  </si>
+  <si>
+    <t>0X11400</t>
+  </si>
+  <si>
+    <t>0X11600</t>
+  </si>
+  <si>
+    <t>0X11800</t>
+  </si>
+  <si>
+    <t>0X11A00</t>
+  </si>
+  <si>
+    <t>0X11C00</t>
+  </si>
+  <si>
+    <t>0X11E00</t>
+  </si>
+  <si>
+    <t>0X12000</t>
+  </si>
+  <si>
+    <t>0X12200</t>
+  </si>
+  <si>
+    <t>0X12400</t>
+  </si>
+  <si>
+    <t>0X12600</t>
+  </si>
+  <si>
+    <t>0X12800</t>
+  </si>
+  <si>
+    <t>0X12A00</t>
+  </si>
+  <si>
+    <t>0X12C00</t>
+  </si>
+  <si>
+    <t>0X12E00</t>
+  </si>
+  <si>
+    <t>0X13000</t>
+  </si>
+  <si>
+    <t>0X13200</t>
+  </si>
+  <si>
+    <t>0X13400</t>
+  </si>
+  <si>
+    <t>0X13600</t>
+  </si>
+  <si>
+    <t>0X13800</t>
+  </si>
+  <si>
+    <t>0X13A00</t>
+  </si>
+  <si>
+    <t>0X13C00</t>
+  </si>
+  <si>
+    <t>0X13E00</t>
+  </si>
+  <si>
+    <t>0X14000</t>
+  </si>
+  <si>
+    <t>0X14200</t>
+  </si>
+  <si>
+    <t>0X14400</t>
+  </si>
+  <si>
+    <t>0X14600</t>
+  </si>
+  <si>
+    <t>0X14800</t>
+  </si>
+  <si>
+    <t>0X14A00</t>
+  </si>
+  <si>
+    <t>0X14C00</t>
+  </si>
+  <si>
+    <t>0X14E00</t>
+  </si>
+  <si>
+    <t>0X15000</t>
+  </si>
+  <si>
+    <t>0X15200</t>
+  </si>
+  <si>
+    <t>0X15400</t>
+  </si>
+  <si>
+    <t>0X15600</t>
+  </si>
+  <si>
+    <t>0X15800</t>
+  </si>
+  <si>
+    <t>0X15A00</t>
+  </si>
+  <si>
+    <t>0X15C00</t>
+  </si>
+  <si>
+    <t>0X15E00</t>
+  </si>
+  <si>
+    <t>0X16000</t>
+  </si>
+  <si>
+    <t>0X16200</t>
+  </si>
+  <si>
+    <t>0X16400</t>
+  </si>
+  <si>
+    <t>0X16600</t>
+  </si>
+  <si>
+    <t>0X16800</t>
+  </si>
+  <si>
+    <t>0X16A00</t>
+  </si>
+  <si>
+    <t>0X16C00</t>
+  </si>
+  <si>
+    <t>0X16E00</t>
+  </si>
+  <si>
+    <t>0X17000</t>
+  </si>
+  <si>
+    <t>0X17200</t>
+  </si>
+  <si>
+    <t>0X17400</t>
+  </si>
+  <si>
+    <t>0X17600</t>
+  </si>
+  <si>
+    <t>0X17800</t>
+  </si>
+  <si>
+    <t>0X17A00</t>
+  </si>
+  <si>
+    <t>0X17C00</t>
+  </si>
+  <si>
+    <t>0X17E00</t>
+  </si>
+  <si>
+    <t>0X18000</t>
+  </si>
+  <si>
+    <t>0X18200</t>
+  </si>
+  <si>
+    <t>0X18400</t>
+  </si>
+  <si>
+    <t>0X18600</t>
+  </si>
+  <si>
+    <t>0X18800</t>
+  </si>
+  <si>
+    <t>0X18A00</t>
+  </si>
+  <si>
+    <t>0X18C00</t>
+  </si>
+  <si>
+    <t>0X18E00</t>
+  </si>
+  <si>
+    <t>0X19000</t>
+  </si>
+  <si>
+    <t>0X19200</t>
+  </si>
+  <si>
+    <t>0X19400</t>
+  </si>
+  <si>
+    <t>0X19600</t>
+  </si>
+  <si>
+    <t>0X19800</t>
+  </si>
+  <si>
+    <t>0X19A00</t>
+  </si>
+  <si>
+    <t>0X19C00</t>
+  </si>
+  <si>
+    <t>0X19E00</t>
+  </si>
+  <si>
+    <t>0X1A000</t>
+  </si>
+  <si>
+    <t>0X1A200</t>
+  </si>
+  <si>
+    <t>0X1A400</t>
+  </si>
+  <si>
+    <t>0X1A600</t>
+  </si>
+  <si>
+    <t>0X1A800</t>
+  </si>
+  <si>
+    <t>0X1AA00</t>
+  </si>
+  <si>
+    <t>0X1AC00</t>
+  </si>
+  <si>
+    <t>0X1AE00</t>
+  </si>
+  <si>
+    <t>0X1B000</t>
+  </si>
+  <si>
+    <t>0X1B200</t>
+  </si>
+  <si>
+    <t>0X1B400</t>
+  </si>
+  <si>
+    <t>0X1B600</t>
+  </si>
+  <si>
+    <t>0X1B800</t>
+  </si>
+  <si>
+    <t>0X1BA00</t>
+  </si>
+  <si>
+    <t>0X1BC00</t>
+  </si>
+  <si>
+    <t>0X1BE00</t>
+  </si>
+  <si>
+    <t>0X1C000</t>
+  </si>
+  <si>
+    <t>0X1C200</t>
+  </si>
+  <si>
+    <t>0X1C400</t>
+  </si>
+  <si>
+    <t>0X1C600</t>
+  </si>
+  <si>
+    <t>0X1C800</t>
+  </si>
+  <si>
+    <t>0X1CA00</t>
+  </si>
+  <si>
+    <t>0X1CC00</t>
+  </si>
+  <si>
+    <t>0X1CE00</t>
+  </si>
+  <si>
+    <t>0X1D000</t>
+  </si>
+  <si>
+    <t>0X1D200</t>
+  </si>
+  <si>
+    <t>0X1D400</t>
+  </si>
+  <si>
+    <t>0X1D600</t>
+  </si>
+  <si>
+    <t>0X1D800</t>
+  </si>
+  <si>
+    <t>0X1DA00</t>
+  </si>
+  <si>
+    <t>0X1DC00</t>
+  </si>
+  <si>
+    <t>0X1DE00</t>
+  </si>
+  <si>
+    <t>0X1E000</t>
+  </si>
+  <si>
+    <t>0X1E200</t>
+  </si>
+  <si>
+    <t>0X1E400</t>
+  </si>
+  <si>
+    <t>0X1E600</t>
+  </si>
+  <si>
+    <t>0X1E800</t>
+  </si>
+  <si>
+    <t>0X1EA00</t>
+  </si>
+  <si>
+    <t>0X1EC00</t>
+  </si>
+  <si>
+    <t>0X1EE00</t>
+  </si>
+  <si>
+    <t>0X1F000</t>
+  </si>
+  <si>
+    <t>0X1F200</t>
+  </si>
+  <si>
+    <t>0X1F400</t>
+  </si>
+  <si>
+    <t>0X1F600</t>
+  </si>
+  <si>
+    <t>All possible sprite addresses and their index in _bESpriteAllocTable</t>
   </si>
 </sst>
 </file>
@@ -733,7 +1142,7 @@
         <v>8000</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -760,7 +1169,7 @@
         <v>8000</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F3">
         <f>D3/8000</f>
@@ -790,7 +1199,7 @@
         <v>48000</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F4">
         <v>6</v>
@@ -819,7 +1228,7 @@
         <v>48000</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F5">
         <v>6</v>
@@ -848,7 +1257,7 @@
         <v>48000</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F6">
         <f>D6/8000</f>
@@ -923,7 +1332,7 @@
         <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -943,7 +1352,7 @@
         <v>8191</v>
       </c>
       <c r="F2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -993,7 +1402,7 @@
         <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -1014,7 +1423,7 @@
         <v>8191</v>
       </c>
       <c r="F2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1064,7 +1473,7 @@
         <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -1085,7 +1494,7 @@
         <v>8191</v>
       </c>
       <c r="F2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1135,7 +1544,7 @@
         <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -1156,7 +1565,7 @@
         <v>3586</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1206,7 +1615,7 @@
         <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -1227,7 +1636,7 @@
         <v>5123</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1277,7 +1686,7 @@
         <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -1298,7 +1707,7 @@
         <v>3723</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1348,7 +1757,7 @@
         <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -1368,7 +1777,7 @@
         <v>3093</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1418,7 +1827,7 @@
         <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -1439,7 +1848,7 @@
         <v>6127</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1489,7 +1898,7 @@
         <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -1510,7 +1919,7 @@
         <v>8191</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1524,7 +1933,7 @@
     </row>
     <row r="34" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M34" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1565,7 +1974,7 @@
         <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -1586,12 +1995,12 @@
         <v>1586</v>
       </c>
       <c r="F2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B3">
         <f>B4-E3</f>
@@ -1608,12 +2017,12 @@
         <v>186</v>
       </c>
       <c r="F3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B4">
         <f>8192-E4</f>
@@ -1630,7 +2039,7 @@
         <v>35</v>
       </c>
       <c r="F4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1683,16 +2092,16 @@
         <v>23</v>
       </c>
       <c r="F1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" t="s">
         <v>66</v>
       </c>
-      <c r="H1" t="s">
-        <v>68</v>
-      </c>
       <c r="I1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -1727,7 +2136,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B3">
         <f>G2+1</f>
@@ -1758,7 +2167,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B4">
         <f>G3+1</f>
@@ -1832,16 +2241,16 @@
         <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -1876,7 +2285,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B3">
         <f>G2+1</f>
@@ -1921,7 +2330,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8A806B9-8F96-4CFC-8F80-C6046C4BB66C}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -2083,7 +2492,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2149,47 +2558,9 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4">
-        <f>B3+ E3+1</f>
-        <v>3782</v>
-      </c>
-      <c r="C4">
-        <v>42</v>
-      </c>
-      <c r="D4">
-        <v>20</v>
-      </c>
-      <c r="E4">
-        <f t="shared" ref="E4" si="2">C4*D4</f>
-        <v>840</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5">
-        <f>B4+ E4+1</f>
-        <v>4623</v>
-      </c>
-      <c r="C5">
-        <v>12</v>
-      </c>
-      <c r="D5">
-        <v>256</v>
-      </c>
-      <c r="E5">
-        <f t="shared" ref="E5" si="3">C5*D5</f>
-        <v>3072</v>
-      </c>
-    </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -2198,7 +2569,7 @@
       </c>
       <c r="E13">
         <f>SUM(E2:E11)</f>
-        <v>7692</v>
+        <v>3780</v>
       </c>
     </row>
   </sheetData>
@@ -2242,7 +2613,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -2298,7 +2669,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -2347,7 +2718,7 @@
         <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -2420,7 +2791,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B5">
         <f>B4+ E4+1</f>
@@ -2443,7 +2814,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -2473,7 +2844,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C9D07F7-AEFD-4D2F-97E3-087A93BF23D8}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -2500,10 +2871,10 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -2512,7 +2883,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -2531,7 +2902,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B3">
         <f>C2</f>
@@ -2551,7 +2922,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B4">
         <f>B3+ C3</f>
@@ -2571,7 +2942,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B5">
         <f>B4+C4</f>
@@ -2591,7 +2962,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B6">
         <f t="shared" ref="B6:B8" si="4">B5+C5</f>
@@ -2611,7 +2982,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B7">
         <f t="shared" si="4"/>
@@ -2631,7 +3002,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B8">
         <f t="shared" si="4"/>
@@ -2651,7 +3022,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C10">
         <f>C8+C5</f>
@@ -2660,7 +3031,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C11">
         <f>SUM(C2:C8)</f>
@@ -2669,7 +3040,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C12">
         <v>129471</v>
@@ -2677,7 +3048,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C13">
         <f>C12-C11</f>
@@ -2687,6 +3058,1115 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72D5F9F0-2373-44BA-8150-CDB117860CA2}">
+  <dimension ref="A1:D136"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="119.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>47</v>
+      </c>
+      <c r="B49" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>48</v>
+      </c>
+      <c r="B50" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>49</v>
+      </c>
+      <c r="B51" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>50</v>
+      </c>
+      <c r="B52" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>51</v>
+      </c>
+      <c r="B53" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>52</v>
+      </c>
+      <c r="B54" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <v>53</v>
+      </c>
+      <c r="B55" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56">
+        <v>54</v>
+      </c>
+      <c r="B56" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <v>55</v>
+      </c>
+      <c r="B57" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A58">
+        <v>56</v>
+      </c>
+      <c r="B58" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <v>57</v>
+      </c>
+      <c r="B59" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A60">
+        <v>58</v>
+      </c>
+      <c r="B60" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A61">
+        <v>59</v>
+      </c>
+      <c r="B61" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A62">
+        <v>60</v>
+      </c>
+      <c r="B62" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A63">
+        <v>61</v>
+      </c>
+      <c r="B63" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A64">
+        <v>62</v>
+      </c>
+      <c r="B64" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A65">
+        <v>63</v>
+      </c>
+      <c r="B65" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A66">
+        <v>64</v>
+      </c>
+      <c r="B66" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A67">
+        <v>65</v>
+      </c>
+      <c r="B67" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A68">
+        <v>66</v>
+      </c>
+      <c r="B68" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A69">
+        <v>67</v>
+      </c>
+      <c r="B69" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A70">
+        <v>68</v>
+      </c>
+      <c r="B70" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A71">
+        <v>69</v>
+      </c>
+      <c r="B71" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A72">
+        <v>70</v>
+      </c>
+      <c r="B72" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A73">
+        <v>71</v>
+      </c>
+      <c r="B73" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A74">
+        <v>72</v>
+      </c>
+      <c r="B74" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A75">
+        <v>73</v>
+      </c>
+      <c r="B75" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A76">
+        <v>74</v>
+      </c>
+      <c r="B76" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A77">
+        <v>75</v>
+      </c>
+      <c r="B77" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A78">
+        <v>76</v>
+      </c>
+      <c r="B78" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A79">
+        <v>77</v>
+      </c>
+      <c r="B79" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A80">
+        <v>78</v>
+      </c>
+      <c r="B80" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A81">
+        <v>79</v>
+      </c>
+      <c r="B81" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A82">
+        <v>80</v>
+      </c>
+      <c r="B82" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A83">
+        <v>81</v>
+      </c>
+      <c r="B83" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A84">
+        <v>82</v>
+      </c>
+      <c r="B84" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A85">
+        <v>83</v>
+      </c>
+      <c r="B85" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A86">
+        <v>84</v>
+      </c>
+      <c r="B86" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A87">
+        <v>85</v>
+      </c>
+      <c r="B87" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A88">
+        <v>86</v>
+      </c>
+      <c r="B88" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A89">
+        <v>87</v>
+      </c>
+      <c r="B89" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A90">
+        <v>88</v>
+      </c>
+      <c r="B90" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A91">
+        <v>89</v>
+      </c>
+      <c r="B91" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A92">
+        <v>90</v>
+      </c>
+      <c r="B92" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A93">
+        <v>91</v>
+      </c>
+      <c r="B93" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A94">
+        <v>92</v>
+      </c>
+      <c r="B94" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A95">
+        <v>93</v>
+      </c>
+      <c r="B95" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A96">
+        <v>94</v>
+      </c>
+      <c r="B96" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A97">
+        <v>95</v>
+      </c>
+      <c r="B97" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A98">
+        <v>96</v>
+      </c>
+      <c r="B98" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A99">
+        <v>97</v>
+      </c>
+      <c r="B99" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A100">
+        <v>98</v>
+      </c>
+      <c r="B100" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A101">
+        <v>99</v>
+      </c>
+      <c r="B101" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A102">
+        <v>100</v>
+      </c>
+      <c r="B102" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A103">
+        <v>101</v>
+      </c>
+      <c r="B103" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A104">
+        <v>102</v>
+      </c>
+      <c r="B104" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A105">
+        <v>103</v>
+      </c>
+      <c r="B105" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A106">
+        <v>104</v>
+      </c>
+      <c r="B106" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A107">
+        <v>105</v>
+      </c>
+      <c r="B107" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A108">
+        <v>106</v>
+      </c>
+      <c r="B108" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A109">
+        <v>107</v>
+      </c>
+      <c r="B109" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A110">
+        <v>108</v>
+      </c>
+      <c r="B110" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A111">
+        <v>109</v>
+      </c>
+      <c r="B111" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A112">
+        <v>110</v>
+      </c>
+      <c r="B112" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A113">
+        <v>111</v>
+      </c>
+      <c r="B113" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A114">
+        <v>112</v>
+      </c>
+      <c r="B114" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A115">
+        <v>113</v>
+      </c>
+      <c r="B115" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A116">
+        <v>114</v>
+      </c>
+      <c r="B116" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A117">
+        <v>115</v>
+      </c>
+      <c r="B117" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A118">
+        <v>116</v>
+      </c>
+      <c r="B118" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A119">
+        <v>117</v>
+      </c>
+      <c r="B119" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A120">
+        <v>118</v>
+      </c>
+      <c r="B120" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A121">
+        <v>119</v>
+      </c>
+      <c r="B121" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A122">
+        <v>120</v>
+      </c>
+      <c r="B122" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A123">
+        <v>121</v>
+      </c>
+      <c r="B123" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A124">
+        <v>122</v>
+      </c>
+      <c r="B124" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A125">
+        <v>123</v>
+      </c>
+      <c r="B125" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A126">
+        <v>124</v>
+      </c>
+      <c r="B126" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A127">
+        <v>125</v>
+      </c>
+      <c r="B127" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A128">
+        <v>126</v>
+      </c>
+      <c r="B128" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A129">
+        <v>127</v>
+      </c>
+      <c r="B129" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A130">
+        <v>128</v>
+      </c>
+      <c r="B130" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A131">
+        <v>129</v>
+      </c>
+      <c r="B131" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A132">
+        <v>130</v>
+      </c>
+      <c r="B132" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A133">
+        <v>131</v>
+      </c>
+      <c r="B133" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A134">
+        <v>132</v>
+      </c>
+      <c r="B134" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A135">
+        <v>133</v>
+      </c>
+      <c r="B135" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A136">
+        <v>134</v>
+      </c>
+      <c r="B136" t="s">
+        <v>216</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -2736,18 +4216,18 @@
         <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -2763,7 +4243,7 @@
         <v>7470</v>
       </c>
       <c r="F2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G2" t="str">
         <f>DEC2HEX(HEX2DEC("A000"))</f>
@@ -2776,7 +4256,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B3">
         <f>C2</f>
@@ -2803,7 +4283,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B4">
         <f>B3+E3</f>
@@ -2836,7 +4316,7 @@
     <row r="6" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="7" spans="1:8" ht="253" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
@@ -2887,7 +4367,7 @@
         <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -2908,7 +4388,7 @@
         <v>8191</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -2959,7 +4439,7 @@
         <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -2980,7 +4460,7 @@
         <v>8191</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -3031,21 +4511,21 @@
         <v>23</v>
       </c>
       <c r="F1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" t="s">
         <v>66</v>
       </c>
-      <c r="H1" t="s">
-        <v>68</v>
-      </c>
       <c r="I1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -3078,7 +4558,7 @@
         <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -3086,7 +4566,7 @@
         <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -3094,7 +4574,7 @@
         <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -3108,7 +4588,7 @@
     </row>
     <row r="13" spans="1:9" ht="145" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -3149,7 +4629,7 @@
         <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -3170,7 +4650,7 @@
         <v>8191</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -3220,7 +4700,7 @@
         <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -3241,7 +4721,7 @@
         <v>6696</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Now using faster multiplier in cel to vera
</commit_message>
<xml_diff>
--- a/docs/allocation.xlsx
+++ b/docs/allocation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E53819-EF13-4656-9259-5A52F4540A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7487825F-C4D9-44BD-A5BB-FF49E80374C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" firstSheet="10" activeTab="25" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" firstSheet="13" activeTab="24" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic (Bank 0x13 - 0x26)" sheetId="2" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="221">
   <si>
     <t>Type</t>
   </si>
@@ -726,6 +726,9 @@
   </si>
   <si>
     <t>All possible sprite addresses and their index in _bESpriteAllocTable</t>
+  </si>
+  <si>
+    <t>Multiplier Output</t>
   </si>
 </sst>
 </file>
@@ -2886,10 +2889,10 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C9D07F7-AEFD-4D2F-97E3-087A93BF23D8}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2940,7 +2943,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="str">
-        <f t="shared" ref="E2:E7" si="0">DEC2HEX(HEX2DEC(D2)+C2-1)</f>
+        <f t="shared" ref="E2:E8" si="0">DEC2HEX(HEX2DEC(D2)+C2-1)</f>
         <v>95FF</v>
       </c>
     </row>
@@ -2956,7 +2959,7 @@
         <v>13440</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D7" si="1">DEC2HEX(B2 + C2)</f>
+        <f t="shared" ref="D3:D8" si="1">DEC2HEX(B2 + C2)</f>
         <v>9600</v>
       </c>
       <c r="E3" t="str">
@@ -2966,136 +2969,156 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>220</v>
       </c>
       <c r="B4">
         <f>B3+ C3</f>
         <v>51840</v>
       </c>
       <c r="C4">
-        <v>128</v>
+        <v>2</v>
       </c>
       <c r="D4" t="str">
-        <f t="shared" ref="D4" si="2">DEC2HEX(B3 + C3)</f>
+        <f>DEC2HEX(B3 + C3)</f>
         <v>CA80</v>
       </c>
       <c r="E4" t="str">
-        <f t="shared" ref="E4" si="3">DEC2HEX(HEX2DEC(D4)+C4-1)</f>
-        <v>CAFF</v>
+        <f>DEC2HEX(HEX2DEC(D4)+C4-1)</f>
+        <v>CA81</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>53</v>
       </c>
       <c r="B5">
-        <f>B4+C4</f>
-        <v>51968</v>
+        <f>B4+ C4</f>
+        <v>51842</v>
       </c>
       <c r="C5">
-        <v>1280</v>
+        <v>126</v>
       </c>
       <c r="D5" t="str">
         <f>DEC2HEX(B4 + C4)</f>
+        <v>CA82</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" ref="E5" si="2">DEC2HEX(HEX2DEC(D5)+C5-1)</f>
+        <v>CAFF</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6">
+        <f>B5+C5</f>
+        <v>51968</v>
+      </c>
+      <c r="C6">
+        <v>1280</v>
+      </c>
+      <c r="D6" t="str">
+        <f>DEC2HEX(B5 + C5)</f>
         <v>CB00</v>
       </c>
-      <c r="E5" t="str">
+      <c r="E6" t="str">
         <f t="shared" si="0"/>
         <v>CFFF</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>72</v>
       </c>
-      <c r="B6">
-        <f t="shared" ref="B6:B8" si="4">B5+C5</f>
+      <c r="B7">
+        <f t="shared" ref="B7:B9" si="3">B6+C6</f>
         <v>53248</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <v>2560</v>
       </c>
-      <c r="D6" t="str">
+      <c r="D7" t="str">
         <f t="shared" si="1"/>
         <v>D000</v>
       </c>
-      <c r="E6" t="str">
+      <c r="E7" t="str">
         <f t="shared" si="0"/>
         <v>D9FF</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>73</v>
       </c>
-      <c r="B7">
-        <f t="shared" si="4"/>
+      <c r="B8">
+        <f t="shared" si="3"/>
         <v>55808</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>4096</v>
       </c>
-      <c r="D7" t="str">
+      <c r="D8" t="str">
         <f t="shared" si="1"/>
         <v>DA00</v>
       </c>
-      <c r="E7" t="str">
+      <c r="E8" t="str">
         <f t="shared" si="0"/>
         <v>E9FF</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>77</v>
       </c>
-      <c r="B8">
-        <f t="shared" si="4"/>
+      <c r="B9">
+        <f t="shared" si="3"/>
         <v>59904</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <v>69120</v>
       </c>
-      <c r="D8" t="str">
-        <f t="shared" ref="D8" si="5">DEC2HEX(B7 + C7)</f>
+      <c r="D9" t="str">
+        <f t="shared" ref="D9" si="4">DEC2HEX(B8 + C8)</f>
         <v>EA00</v>
       </c>
-      <c r="E8" t="str">
-        <f t="shared" ref="E8" si="6">DEC2HEX(HEX2DEC(D8)+C8-1)</f>
+      <c r="E9" t="str">
+        <f t="shared" ref="E9" si="5">DEC2HEX(HEX2DEC(D9)+C9-1)</f>
         <v>1F7FF</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B10" t="s">
-        <v>80</v>
-      </c>
-      <c r="C10">
-        <f>C8+C5</f>
-        <v>70400</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="C11">
-        <f>SUM(C2:C8)</f>
-        <v>129024</v>
+        <f>C9+C6</f>
+        <v>70400</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C12">
-        <v>129471</v>
+        <f>SUM(C2:C9)</f>
+        <v>129024</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13">
+        <v>129471</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
         <v>76</v>
       </c>
-      <c r="C13">
-        <f>C12-C11</f>
+      <c r="C14">
+        <f>C13-C12</f>
         <v>447</v>
       </c>
     </row>
@@ -3109,7 +3132,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72D5F9F0-2373-44BA-8150-CDB117860CA2}">
   <dimension ref="A1:D136"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>

</xml_diff>